<commit_message>
Mission 5. Prepearements. Scene 2
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="m01" sheetId="4" r:id="rId1"/>
     <sheet name="m02" sheetId="1" r:id="rId2"/>
     <sheet name="m03" sheetId="2" r:id="rId3"/>
     <sheet name="m04" sheetId="3" r:id="rId4"/>
+    <sheet name="m05" sheetId="5" r:id="rId5"/>
+    <sheet name="Лист2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'m05'!$A$1:$C$92</definedName>
+  </definedNames>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="813">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -1901,6 +1906,561 @@
   </si>
   <si>
     <t>DX_M01_0320_luc</t>
+  </si>
+  <si>
+    <t>DX_M05_0000_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0010_dispatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0020_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0030_dispatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0040_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0050_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0060_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0070_alaric</t>
+  </si>
+  <si>
+    <t>DX_M05_0080_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0100_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0110_smuggler1</t>
+  </si>
+  <si>
+    <t>DX_M05_0120_smuggler2</t>
+  </si>
+  <si>
+    <t>DX_M05_0130_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0140_smuggler3</t>
+  </si>
+  <si>
+    <t>DX_M05_0150_smuggler2</t>
+  </si>
+  <si>
+    <t>DX_M05_0160_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0170_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0180_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0190_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0200_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0210_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0220_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0230_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0240_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0300_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0310_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0320_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0330_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0340_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0350_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0360_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0370_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0380_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0390_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0400_clark</t>
+  </si>
+  <si>
+    <t>DX_M05_0410_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0420_trader</t>
+  </si>
+  <si>
+    <t>DX_M05_0430_clark</t>
+  </si>
+  <si>
+    <t>DX_M05_0440_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0450_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0460_trader</t>
+  </si>
+  <si>
+    <t>DX_M05_0470_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0480_trader</t>
+  </si>
+  <si>
+    <t>DX_M05_0490_trader</t>
+  </si>
+  <si>
+    <t>DX_M05_0500_trader</t>
+  </si>
+  <si>
+    <t>DX_M05_0510_clark</t>
+  </si>
+  <si>
+    <t>DX_M05_0540_trader</t>
+  </si>
+  <si>
+    <t>DX_M05_0550_mandrake</t>
+  </si>
+  <si>
+    <t>DX_M05_0560_trader</t>
+  </si>
+  <si>
+    <t>DX_M05_0570_clark</t>
+  </si>
+  <si>
+    <t>DX_M05_0580_clark</t>
+  </si>
+  <si>
+    <t>DX_M05_0590_clark</t>
+  </si>
+  <si>
+    <t>DX_M05_0600_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0610_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0620_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0630_mandrake</t>
+  </si>
+  <si>
+    <t>DX_M05_0640_mandrake</t>
+  </si>
+  <si>
+    <t>DX_M05_0650_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0660_mandrake</t>
+  </si>
+  <si>
+    <t>DX_M05_0670_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0680_mandrake</t>
+  </si>
+  <si>
+    <t>DX_M05_0690_mandrake</t>
+  </si>
+  <si>
+    <t>DX_M05_0700_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0710_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0720_police</t>
+  </si>
+  <si>
+    <t>DX_M05_0730_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0740_police</t>
+  </si>
+  <si>
+    <t>DX_M05_0750_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0760_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0770_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0780_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0790_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0800_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0810_police</t>
+  </si>
+  <si>
+    <t>DX_M05_0820_assassin</t>
+  </si>
+  <si>
+    <t>DX_M05_0840_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0850_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0860_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0870_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0880_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0890_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0900_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0910_tilton</t>
+  </si>
+  <si>
+    <t>DX_M05_0920_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0930_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0940_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0950_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0960_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M05_0970_trent</t>
+  </si>
+  <si>
+    <t>0x9A36BACE</t>
+  </si>
+  <si>
+    <t>0xBCDD11CB</t>
+  </si>
+  <si>
+    <t>0x9A36F2CC</t>
+  </si>
+  <si>
+    <t>0xBA36F6CD</t>
+  </si>
+  <si>
+    <t>0xB8D873CB</t>
+  </si>
+  <si>
+    <t>0xBA362ECB</t>
+  </si>
+  <si>
+    <t>0x85268801</t>
+  </si>
+  <si>
+    <t>0x84DB6DCB</t>
+  </si>
+  <si>
+    <t>0x90078A01</t>
+  </si>
+  <si>
+    <t>0xA5D3FDCF</t>
+  </si>
+  <si>
+    <t>0x91FF8401</t>
+  </si>
+  <si>
+    <t>0xBDDD11CF</t>
+  </si>
+  <si>
+    <t>0x91B78601</t>
+  </si>
+  <si>
+    <t>0x91A3870B</t>
+  </si>
+  <si>
+    <t>0x9A222BC0</t>
+  </si>
+  <si>
+    <t>0x8CCD2DC9</t>
+  </si>
+  <si>
+    <t>0xB4838B4B</t>
+  </si>
+  <si>
+    <t>0x9133830B</t>
+  </si>
+  <si>
+    <t>0xBE32F78C</t>
+  </si>
+  <si>
+    <t>0xBBCF48C1</t>
+  </si>
+  <si>
+    <t>0x9DF06201</t>
+  </si>
+  <si>
+    <t>0x9DE4630B</t>
+  </si>
+  <si>
+    <t>0x8E3E0F8C</t>
+  </si>
+  <si>
+    <t>0xB8086841</t>
+  </si>
+  <si>
+    <t>0x9BCE24CA</t>
+  </si>
+  <si>
+    <t>0xB8D06E41</t>
+  </si>
+  <si>
+    <t>0x9BCE6CC8</t>
+  </si>
+  <si>
+    <t>0x8A3B6D8C</t>
+  </si>
+  <si>
+    <t>0x99648749</t>
+  </si>
+  <si>
+    <t>0x9864874D</t>
+  </si>
+  <si>
+    <t>0x9BDAB5C4</t>
+  </si>
+  <si>
+    <t>0x9684870A</t>
+  </si>
+  <si>
+    <t>0x9BDAFDC6</t>
+  </si>
+  <si>
+    <t>0x94848702</t>
+  </si>
+  <si>
+    <t>0x93E4870B</t>
+  </si>
+  <si>
+    <t>0xBBDA21C1</t>
+  </si>
+  <si>
+    <t>0x9BDA6DC2</t>
+  </si>
+  <si>
+    <t>0x8B3B6D88</t>
+  </si>
+  <si>
+    <t>0x9064394C</t>
+  </si>
+  <si>
+    <t>0xB0643D4D</t>
+  </si>
+  <si>
+    <t>0x9065C142</t>
+  </si>
+  <si>
+    <t>0xAC857A04</t>
+  </si>
+  <si>
+    <t>0x95853BC6</t>
+  </si>
+  <si>
+    <t>0xACCD7804</t>
+  </si>
+  <si>
+    <t>0x9B8626CA</t>
+  </si>
+  <si>
+    <t>0xBB8622CB</t>
+  </si>
+  <si>
+    <t>0x90651944</t>
+  </si>
+  <si>
+    <t>0xB9687F0E</t>
+  </si>
+  <si>
+    <t>0xB97C7E04</t>
+  </si>
+  <si>
+    <t>0x9B92B7C4</t>
+  </si>
+  <si>
+    <t>0xB8847004</t>
+  </si>
+  <si>
+    <t>0x8D3E0F80</t>
+  </si>
+  <si>
+    <t>0xBB92FBC7</t>
+  </si>
+  <si>
+    <t>0x9071504C</t>
+  </si>
+  <si>
+    <t>0xB8147404</t>
+  </si>
+  <si>
+    <t>0x9B926FC2</t>
+  </si>
+  <si>
+    <t>0xB0711C4F</t>
+  </si>
+  <si>
+    <t>0x9B5F48C0</t>
+  </si>
+  <si>
+    <t>0xAE53FD89</t>
+  </si>
+  <si>
+    <t>0x9B5EB0CE</t>
+  </si>
+  <si>
+    <t>0xB65D1189</t>
+  </si>
+  <si>
+    <t>0x9B5EF8CC</t>
+  </si>
+  <si>
+    <t>0x9E5F0589</t>
+  </si>
+  <si>
+    <t>0x9B5E20CA</t>
+  </si>
+  <si>
+    <t>0xA6597989</t>
+  </si>
+  <si>
+    <t>0x9B5E68C8</t>
+  </si>
+  <si>
+    <t>0xBB5E6CC9</t>
+  </si>
+  <si>
+    <t>0x9F5F058D</t>
+  </si>
+  <si>
+    <t>0x9B4A21C0</t>
+  </si>
+  <si>
+    <t>0xA759798D</t>
+  </si>
+  <si>
+    <t>0x9B4A69C2</t>
+  </si>
+  <si>
+    <t>0x8F5B6D8D</t>
+  </si>
+  <si>
+    <t>0x9B174AC0</t>
+  </si>
+  <si>
+    <t>0xAC53FD81</t>
+  </si>
+  <si>
+    <t>0x9B16B2CE</t>
+  </si>
+  <si>
+    <t>0xB45D1181</t>
+  </si>
+  <si>
+    <t>0x87C47F48</t>
+  </si>
+  <si>
+    <t>0x9B1622CA</t>
+  </si>
+  <si>
+    <t>0xA7C752C9</t>
+  </si>
+  <si>
+    <t>0x87C69209</t>
+  </si>
+  <si>
+    <t>0xBB166EC9</t>
+  </si>
+  <si>
+    <t>0xBB034FCB</t>
+  </si>
+  <si>
+    <t>0xA1A2C847</t>
+  </si>
+  <si>
+    <t>0xBB02B7C5</t>
+  </si>
+  <si>
+    <t>0x9B02FBC6</t>
+  </si>
+  <si>
+    <t>0xBB02FFC7</t>
+  </si>
+  <si>
+    <t>0xB30E9409</t>
+  </si>
+  <si>
+    <t>0xBB0227C1</t>
+  </si>
+  <si>
+    <t>0xB2261489</t>
+  </si>
+  <si>
+    <t>0x8D5B6D85</t>
+  </si>
+  <si>
+    <t>DX_M05_0530_mandrake</t>
+  </si>
+  <si>
+    <t>DX_M05_0520_trader</t>
+  </si>
+  <si>
+    <t>0xAC157E04</t>
+  </si>
+  <si>
+    <t>0x93E53BCB</t>
+  </si>
+  <si>
+    <t>DX_M05_0830_police</t>
+  </si>
+  <si>
+    <t>0xB4CB894B</t>
   </si>
 </sst>
 </file>
@@ -1937,8 +2497,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2235,7 +2802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C62" sqref="C62:C73"/>
     </sheetView>
   </sheetViews>
@@ -2823,7 +3390,7 @@
   <dimension ref="A2:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B12" sqref="B12:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4024,7 +4591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
@@ -5001,4 +5568,1515 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C92"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="3" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B1" t="s">
+        <v>806</v>
+      </c>
+      <c r="C1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>630</v>
+      </c>
+      <c r="B3" t="s">
+        <v>804</v>
+      </c>
+      <c r="C3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>631</v>
+      </c>
+      <c r="B4" t="s">
+        <v>803</v>
+      </c>
+      <c r="C4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B5" t="s">
+        <v>802</v>
+      </c>
+      <c r="C5" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>633</v>
+      </c>
+      <c r="B6" t="s">
+        <v>801</v>
+      </c>
+      <c r="C6" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B7" t="s">
+        <v>800</v>
+      </c>
+      <c r="C7" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>635</v>
+      </c>
+      <c r="B8" t="s">
+        <v>799</v>
+      </c>
+      <c r="C8" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>636</v>
+      </c>
+      <c r="B9" t="s">
+        <v>798</v>
+      </c>
+      <c r="C9" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>637</v>
+      </c>
+      <c r="B10" t="s">
+        <v>797</v>
+      </c>
+      <c r="C10" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>638</v>
+      </c>
+      <c r="B11" t="s">
+        <v>796</v>
+      </c>
+      <c r="C11" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>639</v>
+      </c>
+      <c r="B12" t="s">
+        <v>795</v>
+      </c>
+      <c r="C12" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>640</v>
+      </c>
+      <c r="B13" t="s">
+        <v>794</v>
+      </c>
+      <c r="C13" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>641</v>
+      </c>
+      <c r="B14" t="s">
+        <v>793</v>
+      </c>
+      <c r="C14" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>642</v>
+      </c>
+      <c r="B15" t="s">
+        <v>812</v>
+      </c>
+      <c r="C15" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>643</v>
+      </c>
+      <c r="B16" t="s">
+        <v>792</v>
+      </c>
+      <c r="C16" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>644</v>
+      </c>
+      <c r="B17" t="s">
+        <v>791</v>
+      </c>
+      <c r="C17" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>645</v>
+      </c>
+      <c r="B18" t="s">
+        <v>790</v>
+      </c>
+      <c r="C18" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>646</v>
+      </c>
+      <c r="B19" t="s">
+        <v>789</v>
+      </c>
+      <c r="C19" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>647</v>
+      </c>
+      <c r="B20" t="s">
+        <v>788</v>
+      </c>
+      <c r="C20" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>648</v>
+      </c>
+      <c r="B21" t="s">
+        <v>787</v>
+      </c>
+      <c r="C21" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>649</v>
+      </c>
+      <c r="B22" t="s">
+        <v>786</v>
+      </c>
+      <c r="C22" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>650</v>
+      </c>
+      <c r="B23" t="s">
+        <v>785</v>
+      </c>
+      <c r="C23" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>651</v>
+      </c>
+      <c r="B24" t="s">
+        <v>784</v>
+      </c>
+      <c r="C24" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>652</v>
+      </c>
+      <c r="B25" t="s">
+        <v>783</v>
+      </c>
+      <c r="C25" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>653</v>
+      </c>
+      <c r="B26" t="s">
+        <v>782</v>
+      </c>
+      <c r="C26" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>654</v>
+      </c>
+      <c r="B27" t="s">
+        <v>781</v>
+      </c>
+      <c r="C27" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>655</v>
+      </c>
+      <c r="B28" t="s">
+        <v>780</v>
+      </c>
+      <c r="C28" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>656</v>
+      </c>
+      <c r="B29" t="s">
+        <v>779</v>
+      </c>
+      <c r="C29" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>657</v>
+      </c>
+      <c r="B30" t="s">
+        <v>778</v>
+      </c>
+      <c r="C30" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>658</v>
+      </c>
+      <c r="B31" t="s">
+        <v>777</v>
+      </c>
+      <c r="C31" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>659</v>
+      </c>
+      <c r="B32" t="s">
+        <v>776</v>
+      </c>
+      <c r="C32" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>660</v>
+      </c>
+      <c r="B33" t="s">
+        <v>775</v>
+      </c>
+      <c r="C33" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>661</v>
+      </c>
+      <c r="B34" t="s">
+        <v>774</v>
+      </c>
+      <c r="C34" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>662</v>
+      </c>
+      <c r="B35" t="s">
+        <v>773</v>
+      </c>
+      <c r="C35" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>663</v>
+      </c>
+      <c r="B36" t="s">
+        <v>772</v>
+      </c>
+      <c r="C36" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>664</v>
+      </c>
+      <c r="B37" t="s">
+        <v>771</v>
+      </c>
+      <c r="C37" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>665</v>
+      </c>
+      <c r="B38" t="s">
+        <v>770</v>
+      </c>
+      <c r="C38" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>666</v>
+      </c>
+      <c r="B39" t="s">
+        <v>769</v>
+      </c>
+      <c r="C39" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>667</v>
+      </c>
+      <c r="B40" t="s">
+        <v>768</v>
+      </c>
+      <c r="C40" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>668</v>
+      </c>
+      <c r="B41" t="s">
+        <v>767</v>
+      </c>
+      <c r="C41" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>669</v>
+      </c>
+      <c r="B42" t="s">
+        <v>766</v>
+      </c>
+      <c r="C42" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>670</v>
+      </c>
+      <c r="B43" t="s">
+        <v>765</v>
+      </c>
+      <c r="C43" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>671</v>
+      </c>
+      <c r="B44" t="s">
+        <v>764</v>
+      </c>
+      <c r="C44" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>672</v>
+      </c>
+      <c r="B45" t="s">
+        <v>810</v>
+      </c>
+      <c r="C45" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>673</v>
+      </c>
+      <c r="B46" t="s">
+        <v>763</v>
+      </c>
+      <c r="C46" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>808</v>
+      </c>
+      <c r="B47" t="s">
+        <v>809</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="B48" t="s">
+        <v>810</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>674</v>
+      </c>
+      <c r="B49" t="s">
+        <v>760</v>
+      </c>
+      <c r="C49" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>675</v>
+      </c>
+      <c r="B50" t="s">
+        <v>759</v>
+      </c>
+      <c r="C50" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>676</v>
+      </c>
+      <c r="B51" t="s">
+        <v>758</v>
+      </c>
+      <c r="C51" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>677</v>
+      </c>
+      <c r="B52" t="s">
+        <v>757</v>
+      </c>
+      <c r="C52" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>678</v>
+      </c>
+      <c r="B53" t="s">
+        <v>756</v>
+      </c>
+      <c r="C53" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>679</v>
+      </c>
+      <c r="B54" t="s">
+        <v>755</v>
+      </c>
+      <c r="C54" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>680</v>
+      </c>
+      <c r="B55" t="s">
+        <v>754</v>
+      </c>
+      <c r="C55" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>681</v>
+      </c>
+      <c r="B56" t="s">
+        <v>753</v>
+      </c>
+      <c r="C56" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>682</v>
+      </c>
+      <c r="B57" t="s">
+        <v>752</v>
+      </c>
+      <c r="C57" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>683</v>
+      </c>
+      <c r="B58" t="s">
+        <v>751</v>
+      </c>
+      <c r="C58" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>684</v>
+      </c>
+      <c r="B59" t="s">
+        <v>750</v>
+      </c>
+      <c r="C59" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>685</v>
+      </c>
+      <c r="B60" t="s">
+        <v>749</v>
+      </c>
+      <c r="C60" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>686</v>
+      </c>
+      <c r="B61" t="s">
+        <v>748</v>
+      </c>
+      <c r="C61" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>687</v>
+      </c>
+      <c r="B62" t="s">
+        <v>747</v>
+      </c>
+      <c r="C62" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>688</v>
+      </c>
+      <c r="B63" t="s">
+        <v>746</v>
+      </c>
+      <c r="C63" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>689</v>
+      </c>
+      <c r="B64" t="s">
+        <v>745</v>
+      </c>
+      <c r="C64" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>690</v>
+      </c>
+      <c r="B65" t="s">
+        <v>744</v>
+      </c>
+      <c r="C65" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>691</v>
+      </c>
+      <c r="B66" t="s">
+        <v>743</v>
+      </c>
+      <c r="C66" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>692</v>
+      </c>
+      <c r="B67" t="s">
+        <v>742</v>
+      </c>
+      <c r="C67" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>693</v>
+      </c>
+      <c r="B68" t="s">
+        <v>741</v>
+      </c>
+      <c r="C68" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>694</v>
+      </c>
+      <c r="B69" t="s">
+        <v>740</v>
+      </c>
+      <c r="C69" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>695</v>
+      </c>
+      <c r="B70" t="s">
+        <v>739</v>
+      </c>
+      <c r="C70" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>696</v>
+      </c>
+      <c r="B71" t="s">
+        <v>738</v>
+      </c>
+      <c r="C71" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>697</v>
+      </c>
+      <c r="B72" t="s">
+        <v>737</v>
+      </c>
+      <c r="C72" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>698</v>
+      </c>
+      <c r="B73" t="s">
+        <v>736</v>
+      </c>
+      <c r="C73" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>699</v>
+      </c>
+      <c r="B74" t="s">
+        <v>735</v>
+      </c>
+      <c r="C74" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>700</v>
+      </c>
+      <c r="B75" t="s">
+        <v>734</v>
+      </c>
+      <c r="C75" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>701</v>
+      </c>
+      <c r="B76" t="s">
+        <v>733</v>
+      </c>
+      <c r="C76" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>702</v>
+      </c>
+      <c r="B77" t="s">
+        <v>732</v>
+      </c>
+      <c r="C77" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>811</v>
+      </c>
+      <c r="B78" t="s">
+        <v>812</v>
+      </c>
+      <c r="C78" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>703</v>
+      </c>
+      <c r="B79" t="s">
+        <v>730</v>
+      </c>
+      <c r="C79" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>704</v>
+      </c>
+      <c r="B80" t="s">
+        <v>729</v>
+      </c>
+      <c r="C80" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>705</v>
+      </c>
+      <c r="B81" t="s">
+        <v>728</v>
+      </c>
+      <c r="C81" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>706</v>
+      </c>
+      <c r="B82" t="s">
+        <v>727</v>
+      </c>
+      <c r="C82" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>707</v>
+      </c>
+      <c r="B83" t="s">
+        <v>726</v>
+      </c>
+      <c r="C83" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>708</v>
+      </c>
+      <c r="B84" t="s">
+        <v>725</v>
+      </c>
+      <c r="C84" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>709</v>
+      </c>
+      <c r="B85" t="s">
+        <v>724</v>
+      </c>
+      <c r="C85" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>710</v>
+      </c>
+      <c r="B86" t="s">
+        <v>723</v>
+      </c>
+      <c r="C86" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>711</v>
+      </c>
+      <c r="B87" t="s">
+        <v>722</v>
+      </c>
+      <c r="C87" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>712</v>
+      </c>
+      <c r="B88" t="s">
+        <v>721</v>
+      </c>
+      <c r="C88" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>713</v>
+      </c>
+      <c r="B89" t="s">
+        <v>720</v>
+      </c>
+      <c r="C89" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>714</v>
+      </c>
+      <c r="B90" t="s">
+        <v>719</v>
+      </c>
+      <c r="C90" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>715</v>
+      </c>
+      <c r="B91" t="s">
+        <v>718</v>
+      </c>
+      <c r="C91" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>716</v>
+      </c>
+      <c r="B92" t="s">
+        <v>717</v>
+      </c>
+      <c r="C92" t="s">
+        <v>716</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:B92"/>
+  <sheetViews>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B92" sqref="B1:B92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" t="s">
+        <v>717</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mission 5. Space: first part
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Лист2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'m05'!$A$1:$C$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'m05'!$A$1:$C$94</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="818">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -2461,6 +2461,21 @@
   </si>
   <si>
     <t>0xB4CB894B</t>
+  </si>
+  <si>
+    <t>DX_M05_0005_trent</t>
+  </si>
+  <si>
+    <t>DX_M05_0395_trent</t>
+  </si>
+  <si>
+    <t>0x8B1F4040</t>
+  </si>
+  <si>
+    <t>0xAB426743</t>
+  </si>
+  <si>
+    <t>0xA7C4FF08</t>
   </si>
 </sst>
 </file>
@@ -5572,10 +5587,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="B11" sqref="B11:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5597,1002 +5612,1024 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>629</v>
+        <v>813</v>
       </c>
       <c r="B2" t="s">
-        <v>805</v>
+        <v>816</v>
       </c>
       <c r="C2" t="s">
-        <v>629</v>
+        <v>813</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B4" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C4" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B5" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B6" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B7" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B8" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="C8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B9" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C9" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B10" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C10" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B11" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C11" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B12" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="C12" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B13" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C13" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B14" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C14" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B15" t="s">
-        <v>812</v>
+        <v>793</v>
       </c>
       <c r="C15" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B16" t="s">
-        <v>792</v>
+        <v>817</v>
       </c>
       <c r="C16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B17" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B18" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C18" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B19" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B20" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C20" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B21" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C21" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B22" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C22" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B23" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C23" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B24" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C24" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B25" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C25" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B26" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C26" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B27" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="C27" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B28" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C28" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B29" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C29" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B30" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B31" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C31" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B32" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B33" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C33" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B34" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C34" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B35" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="C35" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>663</v>
+        <v>814</v>
       </c>
       <c r="B36" t="s">
-        <v>772</v>
+        <v>815</v>
       </c>
       <c r="C36" t="s">
-        <v>663</v>
+        <v>814</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B37" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="C37" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B38" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="C38" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B39" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C39" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B40" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C40" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B41" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="C41" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B42" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C42" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B43" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C43" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B44" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C44" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B45" t="s">
-        <v>810</v>
+        <v>765</v>
       </c>
       <c r="C45" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B46" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C46" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>808</v>
+        <v>672</v>
       </c>
       <c r="B47" t="s">
-        <v>809</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>808</v>
+        <v>810</v>
+      </c>
+      <c r="C47" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
-        <v>807</v>
+      <c r="A48" t="s">
+        <v>673</v>
       </c>
       <c r="B48" t="s">
-        <v>810</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>807</v>
+        <v>763</v>
+      </c>
+      <c r="C48" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>674</v>
+        <v>808</v>
       </c>
       <c r="B49" t="s">
-        <v>760</v>
-      </c>
-      <c r="C49" t="s">
-        <v>674</v>
+        <v>809</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>675</v>
+      <c r="A50" s="1" t="s">
+        <v>807</v>
       </c>
       <c r="B50" t="s">
-        <v>759</v>
-      </c>
-      <c r="C50" t="s">
-        <v>675</v>
+        <v>810</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>807</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B51" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C51" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B52" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C52" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B53" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C53" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B54" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="C54" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B55" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C55" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B56" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="C56" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B57" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="C57" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B58" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C58" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B59" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="C59" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B60" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="C60" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B61" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="C61" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B62" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="C62" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B63" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="C63" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B64" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="C64" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B65" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="C65" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B66" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="C66" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B67" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C67" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B68" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C68" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B69" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C69" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B70" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C70" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B71" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C71" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B72" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C72" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B73" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="C73" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B74" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="C74" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B75" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="C75" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B76" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="C76" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B77" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C77" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>811</v>
+        <v>701</v>
       </c>
       <c r="B78" t="s">
-        <v>812</v>
+        <v>733</v>
       </c>
       <c r="C78" t="s">
-        <v>811</v>
+        <v>701</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B79" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C79" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>704</v>
+        <v>811</v>
       </c>
       <c r="B80" t="s">
-        <v>729</v>
+        <v>812</v>
       </c>
       <c r="C80" t="s">
-        <v>704</v>
+        <v>811</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B81" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C81" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B82" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="C82" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B83" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C83" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B84" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C84" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B85" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="C85" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B86" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="C86" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B87" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C87" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B88" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C88" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B89" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="C89" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B90" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C90" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B91" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C91" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>714</v>
+      </c>
+      <c r="B92" t="s">
+        <v>719</v>
+      </c>
+      <c r="C92" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>715</v>
+      </c>
+      <c r="B93" t="s">
+        <v>718</v>
+      </c>
+      <c r="C93" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>716</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B94" t="s">
         <v>717</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C94" t="s">
         <v>716</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mission 6 voices in progress, weapons refactoring
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61D6FE9-9D44-4285-B811-7630522341AF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m01" sheetId="4" r:id="rId1"/>
@@ -16,13 +22,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'m05'!$A$1:$C$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'m06'!$A$1:$D$47</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="913">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -2755,12 +2762,18 @@
   </si>
   <si>
     <t>0x9B92F30A</t>
+  </si>
+  <si>
+    <t>DX_M06_0225_alaric</t>
+  </si>
+  <si>
+    <t>0xA8988D88</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2810,6 +2823,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2857,7 +2873,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2890,9 +2906,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2925,6 +2958,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -3100,7 +3150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3687,7 +3737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4422,7 +4472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4889,7 +4939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5872,7 +5922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6924,17 +6974,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6955,6 +7006,9 @@
       <c r="B2" t="s">
         <v>865</v>
       </c>
+      <c r="C2" t="s">
+        <v>815</v>
+      </c>
       <c r="D2" t="s">
         <v>862</v>
       </c>
@@ -6966,6 +7020,9 @@
       <c r="B3" t="s">
         <v>866</v>
       </c>
+      <c r="C3" t="s">
+        <v>816</v>
+      </c>
       <c r="D3" t="s">
         <v>862</v>
       </c>
@@ -6977,6 +7034,9 @@
       <c r="B4" t="s">
         <v>867</v>
       </c>
+      <c r="C4" t="s">
+        <v>817</v>
+      </c>
       <c r="D4" t="s">
         <v>863</v>
       </c>
@@ -6988,6 +7048,9 @@
       <c r="B5" t="s">
         <v>868</v>
       </c>
+      <c r="C5" t="s">
+        <v>818</v>
+      </c>
       <c r="D5" t="s">
         <v>862</v>
       </c>
@@ -6999,6 +7062,9 @@
       <c r="B6" t="s">
         <v>869</v>
       </c>
+      <c r="C6" t="s">
+        <v>819</v>
+      </c>
       <c r="D6" t="s">
         <v>863</v>
       </c>
@@ -7010,6 +7076,9 @@
       <c r="B7" t="s">
         <v>870</v>
       </c>
+      <c r="C7" t="s">
+        <v>820</v>
+      </c>
       <c r="D7" t="s">
         <v>862</v>
       </c>
@@ -7021,6 +7090,9 @@
       <c r="B8" t="s">
         <v>871</v>
       </c>
+      <c r="C8" t="s">
+        <v>821</v>
+      </c>
       <c r="D8" t="s">
         <v>862</v>
       </c>
@@ -7032,6 +7104,9 @@
       <c r="B9" t="s">
         <v>872</v>
       </c>
+      <c r="C9" t="s">
+        <v>822</v>
+      </c>
       <c r="D9" t="s">
         <v>864</v>
       </c>
@@ -7043,6 +7118,9 @@
       <c r="B10" t="s">
         <v>873</v>
       </c>
+      <c r="C10" t="s">
+        <v>823</v>
+      </c>
       <c r="D10" t="s">
         <v>864</v>
       </c>
@@ -7054,6 +7132,9 @@
       <c r="B11" t="s">
         <v>874</v>
       </c>
+      <c r="C11" t="s">
+        <v>824</v>
+      </c>
       <c r="D11" t="s">
         <v>864</v>
       </c>
@@ -7065,6 +7146,9 @@
       <c r="B12" t="s">
         <v>875</v>
       </c>
+      <c r="C12" t="s">
+        <v>825</v>
+      </c>
       <c r="D12" t="s">
         <v>863</v>
       </c>
@@ -7076,6 +7160,9 @@
       <c r="B13" t="s">
         <v>876</v>
       </c>
+      <c r="C13" t="s">
+        <v>826</v>
+      </c>
       <c r="D13" t="s">
         <v>864</v>
       </c>
@@ -7087,6 +7174,9 @@
       <c r="B14" t="s">
         <v>877</v>
       </c>
+      <c r="C14" t="s">
+        <v>827</v>
+      </c>
       <c r="D14" t="s">
         <v>864</v>
       </c>
@@ -7098,6 +7188,9 @@
       <c r="B15" t="s">
         <v>878</v>
       </c>
+      <c r="C15" t="s">
+        <v>828</v>
+      </c>
       <c r="D15" t="s">
         <v>863</v>
       </c>
@@ -7109,6 +7202,9 @@
       <c r="B16" t="s">
         <v>879</v>
       </c>
+      <c r="C16" t="s">
+        <v>829</v>
+      </c>
       <c r="D16" t="s">
         <v>864</v>
       </c>
@@ -7120,6 +7216,9 @@
       <c r="B17" t="s">
         <v>880</v>
       </c>
+      <c r="C17" t="s">
+        <v>830</v>
+      </c>
       <c r="D17" t="s">
         <v>863</v>
       </c>
@@ -7131,6 +7230,9 @@
       <c r="B18" t="s">
         <v>881</v>
       </c>
+      <c r="C18" t="s">
+        <v>831</v>
+      </c>
       <c r="D18" t="s">
         <v>864</v>
       </c>
@@ -7142,6 +7244,9 @@
       <c r="B19" t="s">
         <v>882</v>
       </c>
+      <c r="C19" t="s">
+        <v>832</v>
+      </c>
       <c r="D19" t="s">
         <v>864</v>
       </c>
@@ -7153,6 +7258,9 @@
       <c r="B20" t="s">
         <v>883</v>
       </c>
+      <c r="C20" t="s">
+        <v>833</v>
+      </c>
       <c r="D20" t="s">
         <v>864</v>
       </c>
@@ -7164,6 +7272,9 @@
       <c r="B21" t="s">
         <v>884</v>
       </c>
+      <c r="C21" t="s">
+        <v>834</v>
+      </c>
       <c r="D21" t="s">
         <v>863</v>
       </c>
@@ -7175,6 +7286,9 @@
       <c r="B22" t="s">
         <v>885</v>
       </c>
+      <c r="C22" t="s">
+        <v>835</v>
+      </c>
       <c r="D22" t="s">
         <v>864</v>
       </c>
@@ -7186,6 +7300,9 @@
       <c r="B23" t="s">
         <v>886</v>
       </c>
+      <c r="C23" t="s">
+        <v>836</v>
+      </c>
       <c r="D23" t="s">
         <v>863</v>
       </c>
@@ -7197,49 +7314,61 @@
       <c r="B24" t="s">
         <v>887</v>
       </c>
+      <c r="C24" t="s">
+        <v>837</v>
+      </c>
       <c r="D24" t="s">
         <v>864</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>838</v>
+        <v>911</v>
       </c>
       <c r="B25" t="s">
-        <v>888</v>
-      </c>
-      <c r="D25" t="s">
-        <v>864</v>
+        <v>912</v>
+      </c>
+      <c r="C25" t="s">
+        <v>911</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B26" t="s">
-        <v>889</v>
+        <v>888</v>
+      </c>
+      <c r="C26" t="s">
+        <v>838</v>
       </c>
       <c r="D26" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B27" t="s">
-        <v>890</v>
+        <v>889</v>
+      </c>
+      <c r="C27" t="s">
+        <v>839</v>
       </c>
       <c r="D27" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B28" t="s">
-        <v>891</v>
+        <v>890</v>
+      </c>
+      <c r="C28" t="s">
+        <v>840</v>
       </c>
       <c r="D28" t="s">
         <v>864</v>
@@ -7247,21 +7376,27 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B29" t="s">
-        <v>892</v>
+        <v>891</v>
+      </c>
+      <c r="C29" t="s">
+        <v>841</v>
       </c>
       <c r="D29" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B30" t="s">
-        <v>893</v>
+        <v>892</v>
+      </c>
+      <c r="C30" t="s">
+        <v>842</v>
       </c>
       <c r="D30" t="s">
         <v>862</v>
@@ -7269,65 +7404,83 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B31" t="s">
-        <v>894</v>
+        <v>893</v>
+      </c>
+      <c r="C31" t="s">
+        <v>843</v>
       </c>
       <c r="D31" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B32" t="s">
-        <v>895</v>
+        <v>894</v>
+      </c>
+      <c r="C32" t="s">
+        <v>844</v>
       </c>
       <c r="D32" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B33" t="s">
-        <v>896</v>
+        <v>895</v>
+      </c>
+      <c r="C33" t="s">
+        <v>845</v>
       </c>
       <c r="D33" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B34" t="s">
-        <v>897</v>
+        <v>896</v>
+      </c>
+      <c r="C34" t="s">
+        <v>846</v>
       </c>
       <c r="D34" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>899</v>
+        <v>847</v>
       </c>
       <c r="B35" t="s">
-        <v>900</v>
+        <v>897</v>
+      </c>
+      <c r="C35" t="s">
+        <v>847</v>
       </c>
       <c r="D35" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>848</v>
+        <v>899</v>
       </c>
       <c r="B36" t="s">
-        <v>898</v>
+        <v>900</v>
+      </c>
+      <c r="C36" t="s">
+        <v>899</v>
       </c>
       <c r="D36" t="s">
         <v>864</v>
@@ -7335,10 +7488,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B37" t="s">
-        <v>901</v>
+        <v>898</v>
+      </c>
+      <c r="C37" t="s">
+        <v>848</v>
       </c>
       <c r="D37" t="s">
         <v>864</v>
@@ -7346,54 +7502,69 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B38" t="s">
-        <v>902</v>
+        <v>901</v>
+      </c>
+      <c r="C38" t="s">
+        <v>849</v>
       </c>
       <c r="D38" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B39" t="s">
-        <v>903</v>
+        <v>902</v>
+      </c>
+      <c r="C39" t="s">
+        <v>850</v>
       </c>
       <c r="D39" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B40" t="s">
-        <v>904</v>
+        <v>903</v>
+      </c>
+      <c r="C40" t="s">
+        <v>851</v>
       </c>
       <c r="D40" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B41" t="s">
-        <v>905</v>
+        <v>904</v>
+      </c>
+      <c r="C41" t="s">
+        <v>852</v>
       </c>
       <c r="D41" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B42" t="s">
-        <v>906</v>
+        <v>905</v>
+      </c>
+      <c r="C42" t="s">
+        <v>853</v>
       </c>
       <c r="D42" t="s">
         <v>864</v>
@@ -7401,10 +7572,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B43" t="s">
-        <v>907</v>
+        <v>906</v>
+      </c>
+      <c r="C43" t="s">
+        <v>854</v>
       </c>
       <c r="D43" t="s">
         <v>864</v>
@@ -7412,10 +7586,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B44" t="s">
-        <v>908</v>
+        <v>907</v>
+      </c>
+      <c r="C44" t="s">
+        <v>855</v>
       </c>
       <c r="D44" t="s">
         <v>864</v>
@@ -7423,10 +7600,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B45" t="s">
-        <v>909</v>
+        <v>908</v>
+      </c>
+      <c r="C45" t="s">
+        <v>856</v>
       </c>
       <c r="D45" t="s">
         <v>864</v>
@@ -7434,16 +7614,34 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>857</v>
+      </c>
+      <c r="B46" t="s">
+        <v>909</v>
+      </c>
+      <c r="C46" t="s">
+        <v>857</v>
+      </c>
+      <c r="D46" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>858</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>910</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C47" t="s">
+        <v>858</v>
+      </c>
+      <c r="D47" t="s">
         <v>863</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D47" xr:uid="{6A5BD865-1C77-4BEF-ABA8-E64BDEFC5E64}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mission 6 Done before prison
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61D6FE9-9D44-4285-B811-7630522341AF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE015DFD-F5F5-4E0D-812B-9B7301107FE4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,14 +22,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'m05'!$A$1:$C$94</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'m06'!$A$1:$D$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'m06'!$A$1:$C$47</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="989">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -2768,6 +2768,234 @@
   </si>
   <si>
     <t>0xA8988D88</t>
+  </si>
+  <si>
+    <t>DX_M06_1010_professor</t>
+  </si>
+  <si>
+    <t>DX_M06_1020_runner</t>
+  </si>
+  <si>
+    <t>DX_M06_1030_runner</t>
+  </si>
+  <si>
+    <t>DX_M06_1040_runner</t>
+  </si>
+  <si>
+    <t>DX_M06_1050_runner</t>
+  </si>
+  <si>
+    <t>DX_M06_1060_runner</t>
+  </si>
+  <si>
+    <t>0x8A205343</t>
+  </si>
+  <si>
+    <t>0xB88B5E43</t>
+  </si>
+  <si>
+    <t>0xB89F5F49</t>
+  </si>
+  <si>
+    <t>0xB8535843</t>
+  </si>
+  <si>
+    <t>0xB8475949</t>
+  </si>
+  <si>
+    <t>0xB81B5A43</t>
+  </si>
+  <si>
+    <t>Хетчер:\nМистер Трент, я жду вас и вашего компаньона баре космопорта планеты Норидж, система Манхеттен. Хетчер.</t>
+  </si>
+  <si>
+    <t>Хетчер:\nДжентльмены, берем курс на линкор Миссури.</t>
+  </si>
+  <si>
+    <t>Т: Зная рейнландцев, они вокруг этой сферы и ученых наверняка военных на каждый астеорид понапихали, пригнали в систему линкор.</t>
+  </si>
+  <si>
+    <t>Хетчер:\nБерите выше, мистер Трент, у них там развернута военная база.</t>
+  </si>
+  <si>
+    <t>Трент:\nТогда, простите, каким образом мы с напарником должны будем с ними справиться? Вы выдадите нам карманную черную дыру?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хетчер:\nНет, она еще проходит стендовые испытания. Я сейчас сброшу вам по контейнеру, подберите их и стыкуемся с Миссури. </t>
+  </si>
+  <si>
+    <t>Хетчер:\nУдачи, джентльмены. Напоминаю, на территории Рейнланда никаких радиопереговоров со мной.</t>
+  </si>
+  <si>
+    <t>Аларик:\nТрент, чтобы увеличить наши шансы, предлагаю разделиться. Встречаемся внутри Сферы.</t>
+  </si>
+  <si>
+    <t>Станция Гамбург:\nПодключен последний аванпост. Внешний периметр замкнут.</t>
+  </si>
+  <si>
+    <t>Аларик:\nУ нас получилось, Трент.</t>
+  </si>
+  <si>
+    <t>Трент:\nТолько теперь внешний периметр закрыт, и назад дороги нет.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аларик:\nТрент, мы входим в зал в котором рейнландцы развернули лабораторию. Артефакты должны быть где-то внутри. </t>
+  </si>
+  <si>
+    <t>Аларик:\nПопробуй пробраться внутрь через шлюзы и найти Роттермана, а я в это время попробую снять или хотя бы ослабить щиты.</t>
+  </si>
+  <si>
+    <t>Трент:\nАларик, тут все задраено. Не пройти.</t>
+  </si>
+  <si>
+    <t>Аларик:\nТрент, есть другой путь, через технические тоннели. Скидываю координаты.</t>
+  </si>
+  <si>
+    <t>Трент:\nАларик, тут что-то непонятное. Какой-то кристалл, вокруг которого летают корабли Кочевников.</t>
+  </si>
+  <si>
+    <t>Аларик:\nПо данным СБА этот кристалл назвали "Номадским зерном". Если кочевники тебя заметят, то из Зерна будут появляться все новые и новые истребители.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аларик:\nВыход должен находиться рядом, но он был автоматически закрыт после активации Зерна. Чтобы система безопасности разблокировала выход необходимо ликвидировать угрозу в этом зале, то есть уничтожить Зерно и все корабли кочевников. </t>
+  </si>
+  <si>
+    <t>Аларик:\nПроблема в том, что если ты сильно нашумишь, наши рейнландские друзья могут перевозбудиться, поэтому действовать надо быстро.</t>
+  </si>
+  <si>
+    <t>Трент:\nЧерт... Ладно, выключаю невидимость и уничтожаю Зерно.</t>
+  </si>
+  <si>
+    <t>Аларик:\nТрент, быстрее, рейнландцы почуяли неладное в этом зале, хотят направить к тебе оперативную группу.</t>
+  </si>
+  <si>
+    <t>Трент:\nОхренеть. Это что же за адская машина?</t>
+  </si>
+  <si>
+    <t>Ассистент:\nФинн, срочно летите к лаборатории! Поднимайте тревогу!</t>
+  </si>
+  <si>
+    <t>Аларик:\nТрент, ну сколько можно возиться? Присоединяйся, щиты уже основательно просели, им осталось недолго.</t>
+  </si>
+  <si>
+    <t>Аларик:\nДело в шляпе, уходим.</t>
+  </si>
+  <si>
+    <t>Хетчер:\nДжентльмены, для успешного завершения миссии осталось совсем немного. Линкор Миссури уже рядом со Сферой. Стыкуйтесь быстрее!</t>
+  </si>
+  <si>
+    <t>Мостик Миссури:\nКанонерки вышли на огневой рубеж!</t>
+  </si>
+  <si>
+    <t>Мостик Миссури:\nВнимание, залп!</t>
+  </si>
+  <si>
+    <t>Хетчер:\nТрент, Миссури не может совершить прыжок. Повреждены двигатели, требуется ремонт.</t>
+  </si>
+  <si>
+    <t>Хетчер:\nЗдесь становится жарко. Вы с должны будете доставить артефакты на нашу базу в Сигма-17 сами. Я выделю вам для прикрытия звено Дельта.</t>
+  </si>
+  <si>
+    <t>Трент:\nПонял вас, выдвигаюсь. Удачи вам здесь.</t>
+  </si>
+  <si>
+    <t>Хетчер:\nСпасибо, Трент. Поверьте, вам она понадобится не меньше.</t>
+  </si>
+  <si>
+    <t>Аларик:\nТрент, я останусь помогу тут.</t>
+  </si>
+  <si>
+    <t>Трент:\nИ только попробуй мне тут помереть.</t>
+  </si>
+  <si>
+    <t>Дельта-Лидер:\nЛидер звена Дельта. Даю координаты прыжковой дыры в Сигма-17.</t>
+  </si>
+  <si>
+    <t>Пилот Анубиса:\nКапитан Сид, цели успешно перехвачены.</t>
+  </si>
+  <si>
+    <t>Сид:\nФиксируйте их и доставьте на борт "Навуходоносора".</t>
+  </si>
+  <si>
+    <t>Трент:\nТеперь бы еще понять где мы.</t>
+  </si>
+  <si>
+    <t>Дельта-Лидер:\nЯ знаю эту систему. Это Кадиз. Территория Корсаров. Здесь есть свободный порт, куда пускают всех кто смог до него добраться. Называется Фрипорт Тринидад. Там можно будет отсидеться. Вот координаты.</t>
+  </si>
+  <si>
+    <t>Трент:\nОкей, идем туда.</t>
+  </si>
+  <si>
+    <t>Дельта-3:\nКомандир, а вы не хотите направиться в более легальное место?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дельта-Лидер:\nВ более легальном месте нас тут же возьмут под стражу за утрату артефактов и в лучшем случае обвинят в шпионаже. И хрен вы отмоетесь. </t>
+  </si>
+  <si>
+    <t>Дельта-Лидер:\nУлетело пять истребителей с артефактами. Вернулись живые все пятеро, но на одном истребителе и без артефактов. И никто в сказочки с Капитаном Сидом не поверит. Я сам не верил когда однажды задерживал попавших в похожую ситуацию.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дельта-Лидер:\nЕсть конечно еще один вариант - напасть на этом истребителе на Навуходоносор, победить там всех узнать координаты базы Ордена, захватить ее и уже с артефактами и высоко поднятой головой торжественно вернуться в систему Манхеттен. </t>
+  </si>
+  <si>
+    <t>Дельта-Лидер:\nКак думаете, мистер Трент, ваш истребитель способен на такие боевые действия?</t>
+  </si>
+  <si>
+    <t>Трент:\nНе-а. Сто процентов. К тому же, хочу напомнить, господа, вы сейчас находитесь на моем корабле, а посему полетим мы туда, куда скажу я. И сейчас мы летим на Тринидад.</t>
+  </si>
+  <si>
+    <t>Роттерман:\nФинн, срочно летите на главную базу, у нас несанкционированный доступ!</t>
+  </si>
+  <si>
+    <t>Финн:\nНеизвестный пилот, внимание, укажите свой идентификационный код.</t>
+  </si>
+  <si>
+    <t>Финн:\nПрофессор, у нас несанкционированный доступ! Неизвестный корабль не отвечает! Включаю всеобщую тревогу!</t>
+  </si>
+  <si>
+    <t>Финн:\nПрофессор, мой аванпост атакован неизвестным пилотом. Всеобщая тревога!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Финн:\nПрофессор, у нас несанкционированный доступ! В вашу зону направляется неизвестный корабль, спасайтесь! </t>
+  </si>
+  <si>
+    <t>Финн:\nДвери не работают... Всему персоналу, всеобщая тревога! Несанкционированный доступ!</t>
+  </si>
+  <si>
+    <t>Станция Гамбург:\nПатруль Омега-4, это станция Гамбург. Обнаружены неполадки на одном из телескопов. Осмотрите его, возможно разрядился генератор.</t>
+  </si>
+  <si>
+    <t>DX_M06_1100_outpost</t>
+  </si>
+  <si>
+    <t>0xB45A03C8</t>
+  </si>
+  <si>
+    <t>DX_M06_1200_hatcher</t>
+  </si>
+  <si>
+    <t>DX_M06_1210_hatcher</t>
+  </si>
+  <si>
+    <t>Хетчер:\nПовреждения критические! Миссури срочно требуется поддержка! Всем истребителям, приказ перехватить торпеды!</t>
+  </si>
+  <si>
+    <t>Хетчер:\nМы получили попадание торпедой!</t>
+  </si>
+  <si>
+    <t>0xA79ACBCD</t>
+  </si>
+  <si>
+    <t>0xB39BC1CD</t>
+  </si>
+  <si>
+    <t>DX_M06_1220_captain</t>
+  </si>
+  <si>
+    <t>Миссури:\nКанонерки израсходовали боеприпасы и покидают поле битвы. Миссури в безопасности.</t>
+  </si>
+  <si>
+    <t>0xBBB2690A</t>
   </si>
 </sst>
 </file>
@@ -2804,7 +3032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -2812,6 +3040,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6975,31 +7206,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D38" sqref="A37:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="156.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>859</v>
       </c>
       <c r="B1" t="s">
         <v>860</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>815</v>
       </c>
@@ -7007,13 +7238,16 @@
         <v>865</v>
       </c>
       <c r="C2" t="s">
-        <v>815</v>
-      </c>
-      <c r="D2" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>96501</v>
+      </c>
+      <c r="E2" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>816</v>
       </c>
@@ -7021,13 +7255,16 @@
         <v>866</v>
       </c>
       <c r="C3" t="s">
-        <v>816</v>
-      </c>
-      <c r="D3" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>96502</v>
+      </c>
+      <c r="E3" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>817</v>
       </c>
@@ -7035,13 +7272,16 @@
         <v>867</v>
       </c>
       <c r="C4" t="s">
-        <v>817</v>
-      </c>
-      <c r="D4" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>96503</v>
+      </c>
+      <c r="E4" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>818</v>
       </c>
@@ -7049,13 +7289,16 @@
         <v>868</v>
       </c>
       <c r="C5" t="s">
-        <v>818</v>
-      </c>
-      <c r="D5" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>96504</v>
+      </c>
+      <c r="E5" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>819</v>
       </c>
@@ -7063,13 +7306,16 @@
         <v>869</v>
       </c>
       <c r="C6" t="s">
-        <v>819</v>
-      </c>
-      <c r="D6" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>96505</v>
+      </c>
+      <c r="E6" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>820</v>
       </c>
@@ -7077,13 +7323,16 @@
         <v>870</v>
       </c>
       <c r="C7" t="s">
-        <v>820</v>
-      </c>
-      <c r="D7" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>96506</v>
+      </c>
+      <c r="E7" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>821</v>
       </c>
@@ -7091,13 +7340,16 @@
         <v>871</v>
       </c>
       <c r="C8" t="s">
-        <v>821</v>
-      </c>
-      <c r="D8" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>96507</v>
+      </c>
+      <c r="E8" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>822</v>
       </c>
@@ -7105,13 +7357,16 @@
         <v>872</v>
       </c>
       <c r="C9" t="s">
-        <v>822</v>
-      </c>
-      <c r="D9" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>96508</v>
+      </c>
+      <c r="E9" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>823</v>
       </c>
@@ -7119,13 +7374,16 @@
         <v>873</v>
       </c>
       <c r="C10" t="s">
-        <v>823</v>
-      </c>
-      <c r="D10" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>96509</v>
+      </c>
+      <c r="E10" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>824</v>
       </c>
@@ -7133,13 +7391,16 @@
         <v>874</v>
       </c>
       <c r="C11" t="s">
-        <v>824</v>
-      </c>
-      <c r="D11" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>96510</v>
+      </c>
+      <c r="E11" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>825</v>
       </c>
@@ -7147,13 +7408,16 @@
         <v>875</v>
       </c>
       <c r="C12" t="s">
-        <v>825</v>
-      </c>
-      <c r="D12" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>96511</v>
+      </c>
+      <c r="E12" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>826</v>
       </c>
@@ -7161,13 +7425,16 @@
         <v>876</v>
       </c>
       <c r="C13" t="s">
-        <v>826</v>
-      </c>
-      <c r="D13" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>96512</v>
+      </c>
+      <c r="E13" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>827</v>
       </c>
@@ -7175,13 +7442,16 @@
         <v>877</v>
       </c>
       <c r="C14" t="s">
-        <v>827</v>
-      </c>
-      <c r="D14" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>96513</v>
+      </c>
+      <c r="E14" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>828</v>
       </c>
@@ -7189,13 +7459,16 @@
         <v>878</v>
       </c>
       <c r="C15" t="s">
-        <v>828</v>
-      </c>
-      <c r="D15" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>96514</v>
+      </c>
+      <c r="E15" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>829</v>
       </c>
@@ -7203,13 +7476,16 @@
         <v>879</v>
       </c>
       <c r="C16" t="s">
-        <v>829</v>
-      </c>
-      <c r="D16" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>96515</v>
+      </c>
+      <c r="E16" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>830</v>
       </c>
@@ -7217,13 +7493,16 @@
         <v>880</v>
       </c>
       <c r="C17" t="s">
-        <v>830</v>
-      </c>
-      <c r="D17" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>96516</v>
+      </c>
+      <c r="E17" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>831</v>
       </c>
@@ -7231,13 +7510,16 @@
         <v>881</v>
       </c>
       <c r="C18" t="s">
-        <v>831</v>
-      </c>
-      <c r="D18" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>96517</v>
+      </c>
+      <c r="E18" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>832</v>
       </c>
@@ -7245,13 +7527,16 @@
         <v>882</v>
       </c>
       <c r="C19" t="s">
-        <v>832</v>
-      </c>
-      <c r="D19" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>96518</v>
+      </c>
+      <c r="E19" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>833</v>
       </c>
@@ -7259,13 +7544,16 @@
         <v>883</v>
       </c>
       <c r="C20" t="s">
-        <v>833</v>
-      </c>
-      <c r="D20" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>96519</v>
+      </c>
+      <c r="E20" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>834</v>
       </c>
@@ -7273,13 +7561,16 @@
         <v>884</v>
       </c>
       <c r="C21" t="s">
-        <v>834</v>
-      </c>
-      <c r="D21" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>96520</v>
+      </c>
+      <c r="E21" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>835</v>
       </c>
@@ -7287,13 +7578,16 @@
         <v>885</v>
       </c>
       <c r="C22" t="s">
-        <v>835</v>
-      </c>
-      <c r="D22" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>96521</v>
+      </c>
+      <c r="E22" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>836</v>
       </c>
@@ -7301,13 +7595,16 @@
         <v>886</v>
       </c>
       <c r="C23" t="s">
-        <v>836</v>
-      </c>
-      <c r="D23" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>96522</v>
+      </c>
+      <c r="E23" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>837</v>
       </c>
@@ -7315,13 +7612,16 @@
         <v>887</v>
       </c>
       <c r="C24" t="s">
-        <v>837</v>
-      </c>
-      <c r="D24" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>96523</v>
+      </c>
+      <c r="E24" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>911</v>
       </c>
@@ -7329,10 +7629,16 @@
         <v>912</v>
       </c>
       <c r="C25" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>864</v>
+      </c>
+      <c r="D25">
+        <v>96524</v>
+      </c>
+      <c r="E25" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>838</v>
       </c>
@@ -7340,13 +7646,16 @@
         <v>888</v>
       </c>
       <c r="C26" t="s">
-        <v>838</v>
-      </c>
-      <c r="D26" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>96525</v>
+      </c>
+      <c r="E26" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>839</v>
       </c>
@@ -7354,13 +7663,16 @@
         <v>889</v>
       </c>
       <c r="C27" t="s">
-        <v>839</v>
-      </c>
-      <c r="D27" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>96526</v>
+      </c>
+      <c r="E27" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>840</v>
       </c>
@@ -7368,13 +7680,16 @@
         <v>890</v>
       </c>
       <c r="C28" t="s">
-        <v>840</v>
-      </c>
-      <c r="D28" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>96527</v>
+      </c>
+      <c r="E28" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>841</v>
       </c>
@@ -7382,13 +7697,16 @@
         <v>891</v>
       </c>
       <c r="C29" t="s">
-        <v>841</v>
-      </c>
-      <c r="D29" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>96528</v>
+      </c>
+      <c r="E29" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>842</v>
       </c>
@@ -7396,13 +7714,16 @@
         <v>892</v>
       </c>
       <c r="C30" t="s">
-        <v>842</v>
-      </c>
-      <c r="D30" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>96529</v>
+      </c>
+      <c r="E30" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>843</v>
       </c>
@@ -7410,13 +7731,16 @@
         <v>893</v>
       </c>
       <c r="C31" t="s">
-        <v>843</v>
-      </c>
-      <c r="D31" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>96530</v>
+      </c>
+      <c r="E31" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>844</v>
       </c>
@@ -7424,13 +7748,16 @@
         <v>894</v>
       </c>
       <c r="C32" t="s">
-        <v>844</v>
-      </c>
-      <c r="D32" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>96531</v>
+      </c>
+      <c r="E32" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>845</v>
       </c>
@@ -7438,13 +7765,16 @@
         <v>895</v>
       </c>
       <c r="C33" t="s">
-        <v>845</v>
-      </c>
-      <c r="D33" t="s">
         <v>862</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>96532</v>
+      </c>
+      <c r="E33" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>846</v>
       </c>
@@ -7452,13 +7782,16 @@
         <v>896</v>
       </c>
       <c r="C34" t="s">
-        <v>846</v>
-      </c>
-      <c r="D34" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>96533</v>
+      </c>
+      <c r="E34" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>847</v>
       </c>
@@ -7466,13 +7799,16 @@
         <v>897</v>
       </c>
       <c r="C35" t="s">
-        <v>847</v>
-      </c>
-      <c r="D35" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>96534</v>
+      </c>
+      <c r="E35" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>899</v>
       </c>
@@ -7480,13 +7816,16 @@
         <v>900</v>
       </c>
       <c r="C36" t="s">
-        <v>899</v>
-      </c>
-      <c r="D36" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>96535</v>
+      </c>
+      <c r="E36" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>848</v>
       </c>
@@ -7494,13 +7833,16 @@
         <v>898</v>
       </c>
       <c r="C37" t="s">
-        <v>848</v>
-      </c>
-      <c r="D37" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>96536</v>
+      </c>
+      <c r="E37" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>849</v>
       </c>
@@ -7508,13 +7850,16 @@
         <v>901</v>
       </c>
       <c r="C38" t="s">
-        <v>849</v>
-      </c>
-      <c r="D38" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>96537</v>
+      </c>
+      <c r="E38" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>850</v>
       </c>
@@ -7522,13 +7867,16 @@
         <v>902</v>
       </c>
       <c r="C39" t="s">
-        <v>850</v>
-      </c>
-      <c r="D39" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>96538</v>
+      </c>
+      <c r="E39" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>851</v>
       </c>
@@ -7536,13 +7884,16 @@
         <v>903</v>
       </c>
       <c r="C40" t="s">
-        <v>851</v>
-      </c>
-      <c r="D40" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>96539</v>
+      </c>
+      <c r="E40" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>852</v>
       </c>
@@ -7550,13 +7901,16 @@
         <v>904</v>
       </c>
       <c r="C41" t="s">
-        <v>852</v>
-      </c>
-      <c r="D41" t="s">
         <v>863</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>96540</v>
+      </c>
+      <c r="E41" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>853</v>
       </c>
@@ -7564,13 +7918,16 @@
         <v>905</v>
       </c>
       <c r="C42" t="s">
-        <v>853</v>
-      </c>
-      <c r="D42" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>96541</v>
+      </c>
+      <c r="E42" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>854</v>
       </c>
@@ -7578,13 +7935,16 @@
         <v>906</v>
       </c>
       <c r="C43" t="s">
-        <v>854</v>
-      </c>
-      <c r="D43" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>96542</v>
+      </c>
+      <c r="E43" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>855</v>
       </c>
@@ -7592,13 +7952,16 @@
         <v>907</v>
       </c>
       <c r="C44" t="s">
-        <v>855</v>
-      </c>
-      <c r="D44" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>96543</v>
+      </c>
+      <c r="E44" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>856</v>
       </c>
@@ -7606,13 +7969,16 @@
         <v>908</v>
       </c>
       <c r="C45" t="s">
-        <v>856</v>
-      </c>
-      <c r="D45" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>96544</v>
+      </c>
+      <c r="E45" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>857</v>
       </c>
@@ -7620,13 +7986,16 @@
         <v>909</v>
       </c>
       <c r="C46" t="s">
-        <v>857</v>
-      </c>
-      <c r="D46" t="s">
         <v>864</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>96545</v>
+      </c>
+      <c r="E46" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>858</v>
       </c>
@@ -7634,14 +8003,188 @@
         <v>910</v>
       </c>
       <c r="C47" t="s">
-        <v>858</v>
-      </c>
-      <c r="D47" t="s">
         <v>863</v>
       </c>
+      <c r="D47">
+        <v>96546</v>
+      </c>
+      <c r="E47" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>913</v>
+      </c>
+      <c r="B48" t="s">
+        <v>919</v>
+      </c>
+      <c r="C48" t="s">
+        <v>864</v>
+      </c>
+      <c r="D48">
+        <v>96547</v>
+      </c>
+      <c r="E48" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>914</v>
+      </c>
+      <c r="B49" t="s">
+        <v>920</v>
+      </c>
+      <c r="C49" t="s">
+        <v>864</v>
+      </c>
+      <c r="D49">
+        <v>96548</v>
+      </c>
+      <c r="E49" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>915</v>
+      </c>
+      <c r="B50" t="s">
+        <v>921</v>
+      </c>
+      <c r="C50" t="s">
+        <v>864</v>
+      </c>
+      <c r="D50">
+        <v>96549</v>
+      </c>
+      <c r="E50" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>916</v>
+      </c>
+      <c r="B51" t="s">
+        <v>922</v>
+      </c>
+      <c r="C51" t="s">
+        <v>864</v>
+      </c>
+      <c r="D51">
+        <v>96550</v>
+      </c>
+      <c r="E51" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>917</v>
+      </c>
+      <c r="B52" t="s">
+        <v>923</v>
+      </c>
+      <c r="C52" t="s">
+        <v>864</v>
+      </c>
+      <c r="D52">
+        <v>96551</v>
+      </c>
+      <c r="E52" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>918</v>
+      </c>
+      <c r="B53" t="s">
+        <v>924</v>
+      </c>
+      <c r="C53" t="s">
+        <v>864</v>
+      </c>
+      <c r="D53">
+        <v>96552</v>
+      </c>
+      <c r="E53" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>978</v>
+      </c>
+      <c r="B54" t="s">
+        <v>979</v>
+      </c>
+      <c r="C54" t="s">
+        <v>864</v>
+      </c>
+      <c r="D54">
+        <v>96553</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>980</v>
+      </c>
+      <c r="B55" t="s">
+        <v>985</v>
+      </c>
+      <c r="C55" t="s">
+        <v>862</v>
+      </c>
+      <c r="D55">
+        <v>96554</v>
+      </c>
+      <c r="E55" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>981</v>
+      </c>
+      <c r="B56" t="s">
+        <v>984</v>
+      </c>
+      <c r="C56" t="s">
+        <v>862</v>
+      </c>
+      <c r="D56">
+        <v>96555</v>
+      </c>
+      <c r="E56" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>986</v>
+      </c>
+      <c r="B57" t="s">
+        <v>988</v>
+      </c>
+      <c r="C57" t="s">
+        <v>864</v>
+      </c>
+      <c r="D57">
+        <v>96556</v>
+      </c>
+      <c r="E57" t="s">
+        <v>987</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D47" xr:uid="{6A5BD865-1C77-4BEF-ABA8-E64BDEFC5E64}"/>
+  <autoFilter ref="A1:C47" xr:uid="{6A5BD865-1C77-4BEF-ABA8-E64BDEFC5E64}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mission 6 gameplay really done
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE015DFD-F5F5-4E0D-812B-9B7301107FE4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D16B77-B124-490E-AA24-9065F17DBA9C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7208,8 +7208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D38" sqref="A37:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mission 6 Eng version completed
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CBCA6B-6EBB-40B1-B48C-147D4A2F1A24}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE42D6BC-167E-478E-A1C0-DD3C8DED5FE9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="1045">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -2996,6 +2996,174 @@
   </si>
   <si>
     <t>Трент:\nЗная рейнландцев, они вокруг этой сферы и ученых наверняка военных на каждый астеорид понапихали, пригнали в систему линкор.</t>
+  </si>
+  <si>
+    <t>Hatcher:\nMr. Trent, I'm waiting for you and your companion on Planet Norwich in the Manhattan System. Hatcher out.</t>
+  </si>
+  <si>
+    <t>Hatcher:\nGentlemen, please set course to Battleship Missouri.</t>
+  </si>
+  <si>
+    <t>Hatcher:\nThat's an understatement, Mr. Trent. In fact, they have a fully deployed military base there.</t>
+  </si>
+  <si>
+    <t>Тrent:\nExcuse me, but how exactly do you expect me and my wingman to deal with that? Are you gonna give us a black hole that can fit in our pockets?</t>
+  </si>
+  <si>
+    <t>Hatcher:\nNo, that device is still being tested. I'll drop a few containers for you, tractor them in and dock with Missouri.</t>
+  </si>
+  <si>
+    <t>Hatcher:\nBest of luck, gentlemen. And remember – maintain radio silence with me once you've reached Rheinland.</t>
+  </si>
+  <si>
+    <t>Alaric:\nTrent, we’ll have a better chance at it if we split up. I'll meet you inside the sphere.</t>
+  </si>
+  <si>
+    <t>Outpost:\nLast outpost is operational. External perimeter is locked down.</t>
+  </si>
+  <si>
+    <t>Аlaric:\nWe made it, Trent!</t>
+  </si>
+  <si>
+    <t>Тrent:\nExcept the outer perimeter is locked down, so there's no longer a way back.</t>
+  </si>
+  <si>
+    <t>Аlaric:\nTrent, we're entering the hall where Rheinlanders deployed their lab. Artifacts should be somewhere inside.</t>
+  </si>
+  <si>
+    <t>Аlaric:\nTry sneaking in through the airlocks and find Rotterman, while I try to take down or weaken the shields.</t>
+  </si>
+  <si>
+    <t>Trent:\nAlaric, it's all sealed down here. I can't get through.</t>
+  </si>
+  <si>
+    <t>Alaric:\nTrent, there's another way, through maintenance vents. I'm sending you the coordinates.</t>
+  </si>
+  <si>
+    <t>Trent:\nAlaric, there's something weird in here. Some kind of crystal, surrounded by Nomad ships.</t>
+  </si>
+  <si>
+    <t>Alaric:\nASF intel says this crystal is called "The Nomad Seed". If Nomads sense your presence, their ships will start pouring out of this thing.</t>
+  </si>
+  <si>
+    <t>Alaric:\nThe exit was somewhere around here, but it was automatically sealed after the Seed activated. In order to unseal it, you need to eliminate all the threats:\nboth the Seed and all Nomad ships.</t>
+  </si>
+  <si>
+    <t>Аlaric:\nThe only problem is, if you make too much noise, our Rheinland friends will join the party. So, you have to act quickly.</t>
+  </si>
+  <si>
+    <t>Trent:\nDammit… Alright, powering off cloak and attacking the Seed.</t>
+  </si>
+  <si>
+    <t>Alaric:\nTrent, hurry up! The Rheinlanders are sensing something’s wrong in that hall. They want to send a group of scouts there.</t>
+  </si>
+  <si>
+    <t>Тrent:\nHoly shit! What the hell is this kind of machine?</t>
+  </si>
+  <si>
+    <t>Assistant:\nFinn, get to the lab immediately! Sound the alarm!</t>
+  </si>
+  <si>
+    <t>Alaric:\nTrent, what's taking you so long? Come here, the shields are almost gone - it won't take much longer.</t>
+  </si>
+  <si>
+    <t>Alaric:\nIt's finished. Let's get out of here.</t>
+  </si>
+  <si>
+    <t>Hatcher:\nGentlemen, we're almost done with this mission. Battleship Missouri is approaching the Sphere. Proceed to dock, quickly!</t>
+  </si>
+  <si>
+    <t>Radar operator:\nGunships at the firing range.</t>
+  </si>
+  <si>
+    <t>Radar operator:\nReady, set... fire!</t>
+  </si>
+  <si>
+    <t>Hatcher:\nTrent, Missouri won't be able to jump. Its engines are damaged and need repairs.</t>
+  </si>
+  <si>
+    <t>Hatcher:\nIt's getting hot here. You’ll have to deliver these artifacts to our base in Sigma-17 on your own. The Delta wing will escort you.</t>
+  </si>
+  <si>
+    <t>Trent:\nAcknowledged, moving out. Good luck out here.</t>
+  </si>
+  <si>
+    <t>Hatcher:\nThanks Trent. Trust me, you'll need it more than I do.</t>
+  </si>
+  <si>
+    <t>Alaric:\nTrent, I'm staying here to help.</t>
+  </si>
+  <si>
+    <t>Trent:\nJust try to stay alive, OK?</t>
+  </si>
+  <si>
+    <t>Delta Wing Leader:\nThis is Delta leader; I'm sending you the coordinates for the Sigma-17 jump hole.</t>
+  </si>
+  <si>
+    <t>Anubis pilot:\nCaptain Syd, targets successfully intercepted.</t>
+  </si>
+  <si>
+    <t>Syd:\nFreeze them and deliver them to Nebuchadnezzar.</t>
+  </si>
+  <si>
+    <t>Trent:\nNow, where the hell are we?</t>
+  </si>
+  <si>
+    <t>Delta Leader:\nI know this system. This is Cadiz, in the Corsair territory. There's a Freeport here that allows anyone to dock, it's called Trinidad Freeport. We can wait there. Sending you the coordinates.</t>
+  </si>
+  <si>
+    <t>Trent:\nSweet, let's go there.</t>
+  </si>
+  <si>
+    <t>Delta 3:\nHey commander, wouldn't you prefer to fly to a slightly more "lawful" place?</t>
+  </si>
+  <si>
+    <t>Delta Leader:\nIn a slightly more "lawful" place, you'd immediately get apprehended for losing the artifacts. And, in the best case, get accused of espionage. Good luck getting out of prison.</t>
+  </si>
+  <si>
+    <t>Delta Leader:\nThink of it this way:\nfive vessels flew out, with artifacts on board. All five came back alive, but on one ship, and without artifacts. No one would ever believe your cute little story about Syd, trust me. I didn't think so either until I was ordered to capture others who ended up in a similar situation.</t>
+  </si>
+  <si>
+    <t>Delta Leader:\nOf course, there's another option - quickly kill everyone on Nebuchadnezzar, steal the coordinates for their secret base, capture it, and come back to Manhattan. Glorious, victorious, and with artifacts in your hands.</t>
+  </si>
+  <si>
+    <t>Delta Leader:\nMr. Trent, is your ship capable of such aggressive maneuvers?</t>
+  </si>
+  <si>
+    <t>Trent:\nRest assure it cannot. By the way, since you gentlemen are on board my ship, let me remind you that you're going to fly where I say. And right now, we're going to Trinidad.</t>
+  </si>
+  <si>
+    <t>Rotterman:\nFinn, we have a security breach, come to the main base immediately!</t>
+  </si>
+  <si>
+    <t>Finn:\nUnidentified pilot, please transmit your ID code immediately.</t>
+  </si>
+  <si>
+    <t>Finn:\nProfessor, we have a breach! The unidentified ship isn’t responding! Activating the alarm!</t>
+  </si>
+  <si>
+    <t>Finn:\nProfessor, my outpost is being attacked by the unknown vessel. Alarm! Alarm!</t>
+  </si>
+  <si>
+    <t>Finn:\nProfessor, we’re being breached! The unknown ship is headed towards you. You must escape!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finn:\nDoors are sealed… To all personnel, this is not a drill! We have a security breach! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamburg Station:\nOmega-4 patrol, this is Hamburg station. We found issues on one of the telescopes. Take a look, maybe its battery is low. </t>
+  </si>
+  <si>
+    <t>Hatcher:\nWe’ve been hit by a torpedo!</t>
+  </si>
+  <si>
+    <t>Hatcher:\nSustained critical damage! Missouri needs immediate assistance! To all fighter wings, your order is to intercept the torpedoes at once!</t>
+  </si>
+  <si>
+    <t>Missouri:\nGunships have exhausted their ammo and are leaving the battlefield. Missouri is safe.</t>
+  </si>
+  <si>
+    <t>Тrent:\nKnowing Rheinland, there’s probably tight guard around each and every asteroid around the sphere, and I bet they stuck a battleship in there.</t>
   </si>
 </sst>
 </file>
@@ -7206,20 +7374,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="5" max="5" width="156.42578125" customWidth="1"/>
+    <col min="5" max="5" width="178.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>859</v>
       </c>
@@ -7230,7 +7399,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>815</v>
       </c>
@@ -7244,10 +7413,13 @@
         <v>96501</v>
       </c>
       <c r="E2" t="s">
+        <v>989</v>
+      </c>
+      <c r="F2" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>816</v>
       </c>
@@ -7261,10 +7433,13 @@
         <v>96502</v>
       </c>
       <c r="E3" t="s">
+        <v>990</v>
+      </c>
+      <c r="F3" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>817</v>
       </c>
@@ -7278,10 +7453,13 @@
         <v>96503</v>
       </c>
       <c r="E4" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F4" t="s">
         <v>988</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>818</v>
       </c>
@@ -7295,10 +7473,13 @@
         <v>96504</v>
       </c>
       <c r="E5" t="s">
+        <v>991</v>
+      </c>
+      <c r="F5" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>819</v>
       </c>
@@ -7312,10 +7493,13 @@
         <v>96505</v>
       </c>
       <c r="E6" t="s">
+        <v>992</v>
+      </c>
+      <c r="F6" t="s">
         <v>928</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>820</v>
       </c>
@@ -7329,10 +7513,13 @@
         <v>96506</v>
       </c>
       <c r="E7" t="s">
+        <v>993</v>
+      </c>
+      <c r="F7" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>821</v>
       </c>
@@ -7346,10 +7533,13 @@
         <v>96507</v>
       </c>
       <c r="E8" t="s">
+        <v>994</v>
+      </c>
+      <c r="F8" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>822</v>
       </c>
@@ -7363,10 +7553,13 @@
         <v>96508</v>
       </c>
       <c r="E9" t="s">
+        <v>995</v>
+      </c>
+      <c r="F9" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>823</v>
       </c>
@@ -7380,10 +7573,13 @@
         <v>96509</v>
       </c>
       <c r="E10" t="s">
+        <v>996</v>
+      </c>
+      <c r="F10" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>824</v>
       </c>
@@ -7397,10 +7593,13 @@
         <v>96510</v>
       </c>
       <c r="E11" t="s">
+        <v>997</v>
+      </c>
+      <c r="F11" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>825</v>
       </c>
@@ -7414,10 +7613,13 @@
         <v>96511</v>
       </c>
       <c r="E12" t="s">
+        <v>998</v>
+      </c>
+      <c r="F12" t="s">
         <v>934</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>826</v>
       </c>
@@ -7431,10 +7633,13 @@
         <v>96512</v>
       </c>
       <c r="E13" t="s">
+        <v>999</v>
+      </c>
+      <c r="F13" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>827</v>
       </c>
@@ -7448,10 +7653,13 @@
         <v>96513</v>
       </c>
       <c r="E14" t="s">
+        <v>1000</v>
+      </c>
+      <c r="F14" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>828</v>
       </c>
@@ -7465,10 +7673,13 @@
         <v>96514</v>
       </c>
       <c r="E15" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F15" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>829</v>
       </c>
@@ -7482,10 +7693,13 @@
         <v>96515</v>
       </c>
       <c r="E16" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F16" t="s">
         <v>938</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>830</v>
       </c>
@@ -7499,10 +7713,13 @@
         <v>96516</v>
       </c>
       <c r="E17" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F17" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>831</v>
       </c>
@@ -7516,10 +7733,13 @@
         <v>96517</v>
       </c>
       <c r="E18" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F18" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>832</v>
       </c>
@@ -7533,10 +7753,13 @@
         <v>96518</v>
       </c>
       <c r="E19" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F19" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>833</v>
       </c>
@@ -7550,10 +7773,13 @@
         <v>96519</v>
       </c>
       <c r="E20" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F20" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>834</v>
       </c>
@@ -7567,10 +7793,13 @@
         <v>96520</v>
       </c>
       <c r="E21" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F21" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>835</v>
       </c>
@@ -7584,10 +7813,13 @@
         <v>96521</v>
       </c>
       <c r="E22" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F22" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>836</v>
       </c>
@@ -7601,10 +7833,13 @@
         <v>96522</v>
       </c>
       <c r="E23" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F23" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>837</v>
       </c>
@@ -7618,10 +7853,13 @@
         <v>96523</v>
       </c>
       <c r="E24" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F24" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>911</v>
       </c>
@@ -7635,10 +7873,13 @@
         <v>96524</v>
       </c>
       <c r="E25" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F25" t="s">
         <v>947</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>838</v>
       </c>
@@ -7652,10 +7893,13 @@
         <v>96525</v>
       </c>
       <c r="E26" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F26" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>839</v>
       </c>
@@ -7669,10 +7913,13 @@
         <v>96526</v>
       </c>
       <c r="E27" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F27" t="s">
         <v>949</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>840</v>
       </c>
@@ -7686,10 +7933,13 @@
         <v>96527</v>
       </c>
       <c r="E28" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F28" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>841</v>
       </c>
@@ -7703,10 +7953,13 @@
         <v>96528</v>
       </c>
       <c r="E29" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F29" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>842</v>
       </c>
@@ -7720,10 +7973,13 @@
         <v>96529</v>
       </c>
       <c r="E30" t="s">
+        <v>1016</v>
+      </c>
+      <c r="F30" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>843</v>
       </c>
@@ -7737,10 +7993,13 @@
         <v>96530</v>
       </c>
       <c r="E31" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F31" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>844</v>
       </c>
@@ -7754,10 +8013,13 @@
         <v>96531</v>
       </c>
       <c r="E32" t="s">
+        <v>1018</v>
+      </c>
+      <c r="F32" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>845</v>
       </c>
@@ -7771,10 +8033,13 @@
         <v>96532</v>
       </c>
       <c r="E33" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F33" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>846</v>
       </c>
@@ -7788,10 +8053,13 @@
         <v>96533</v>
       </c>
       <c r="E34" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F34" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>847</v>
       </c>
@@ -7805,10 +8073,13 @@
         <v>96534</v>
       </c>
       <c r="E35" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F35" t="s">
         <v>957</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>899</v>
       </c>
@@ -7822,10 +8093,13 @@
         <v>96535</v>
       </c>
       <c r="E36" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F36" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>848</v>
       </c>
@@ -7839,10 +8113,13 @@
         <v>96536</v>
       </c>
       <c r="E37" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F37" t="s">
         <v>959</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>849</v>
       </c>
@@ -7856,10 +8133,13 @@
         <v>96537</v>
       </c>
       <c r="E38" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F38" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>850</v>
       </c>
@@ -7873,10 +8153,13 @@
         <v>96538</v>
       </c>
       <c r="E39" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F39" t="s">
         <v>961</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>851</v>
       </c>
@@ -7890,10 +8173,13 @@
         <v>96539</v>
       </c>
       <c r="E40" t="s">
+        <v>1026</v>
+      </c>
+      <c r="F40" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>852</v>
       </c>
@@ -7907,10 +8193,13 @@
         <v>96540</v>
       </c>
       <c r="E41" t="s">
+        <v>1027</v>
+      </c>
+      <c r="F41" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>853</v>
       </c>
@@ -7924,10 +8213,13 @@
         <v>96541</v>
       </c>
       <c r="E42" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F42" t="s">
         <v>964</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>854</v>
       </c>
@@ -7941,10 +8233,13 @@
         <v>96542</v>
       </c>
       <c r="E43" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F43" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>855</v>
       </c>
@@ -7958,10 +8253,13 @@
         <v>96543</v>
       </c>
       <c r="E44" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F44" t="s">
         <v>966</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>856</v>
       </c>
@@ -7975,10 +8273,13 @@
         <v>96544</v>
       </c>
       <c r="E45" t="s">
+        <v>1031</v>
+      </c>
+      <c r="F45" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>857</v>
       </c>
@@ -7992,10 +8293,13 @@
         <v>96545</v>
       </c>
       <c r="E46" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F46" t="s">
         <v>968</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>858</v>
       </c>
@@ -8009,10 +8313,13 @@
         <v>96546</v>
       </c>
       <c r="E47" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F47" t="s">
         <v>969</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>913</v>
       </c>
@@ -8026,10 +8333,13 @@
         <v>96547</v>
       </c>
       <c r="E48" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F48" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>914</v>
       </c>
@@ -8043,10 +8353,13 @@
         <v>96548</v>
       </c>
       <c r="E49" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F49" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>915</v>
       </c>
@@ -8060,10 +8373,13 @@
         <v>96549</v>
       </c>
       <c r="E50" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F50" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>916</v>
       </c>
@@ -8077,10 +8393,13 @@
         <v>96550</v>
       </c>
       <c r="E51" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F51" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>917</v>
       </c>
@@ -8094,10 +8413,13 @@
         <v>96551</v>
       </c>
       <c r="E52" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F52" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>918</v>
       </c>
@@ -8111,10 +8433,13 @@
         <v>96552</v>
       </c>
       <c r="E53" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F53" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>977</v>
       </c>
@@ -8127,11 +8452,14 @@
       <c r="D54">
         <v>96553</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>979</v>
       </c>
@@ -8145,10 +8473,13 @@
         <v>96554</v>
       </c>
       <c r="E55" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F55" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>980</v>
       </c>
@@ -8162,10 +8493,13 @@
         <v>96555</v>
       </c>
       <c r="E56" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F56" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>985</v>
       </c>
@@ -8179,6 +8513,9 @@
         <v>96556</v>
       </c>
       <c r="E57" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F57" t="s">
         <v>986</v>
       </c>
     </row>

</xml_diff>

<commit_message>
After mission 6 fixes, starflier-line anim
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE42D6BC-167E-478E-A1C0-DD3C8DED5FE9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B87350-5660-4CEC-9761-650409056DBA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="1048">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -3164,6 +3164,15 @@
   </si>
   <si>
     <t>Тrent:\nKnowing Rheinland, there’s probably tight guard around each and every asteroid around the sphere, and I bet they stuck a battleship in there.</t>
+  </si>
+  <si>
+    <t>txt eng</t>
+  </si>
+  <si>
+    <t>txt ru</t>
+  </si>
+  <si>
+    <t>string id</t>
   </si>
 </sst>
 </file>
@@ -5342,7 +5351,7 @@
   <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6324,7 +6333,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="A20:C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7376,16 +7387,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="5" max="5" width="178.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="109.42578125" customWidth="1"/>
+    <col min="6" max="6" width="94" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7397,6 +7408,15 @@
       </c>
       <c r="C1" t="s">
         <v>861</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1046</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mission 8. Lair Escape Race complete
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B87350-5660-4CEC-9761-650409056DBA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B045911E-648C-4FA1-9007-D1EA3A2845B2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m01" sheetId="4" r:id="rId1"/>
@@ -19,17 +19,18 @@
     <sheet name="m04" sheetId="3" r:id="rId4"/>
     <sheet name="m05" sheetId="5" r:id="rId5"/>
     <sheet name="m06" sheetId="6" r:id="rId6"/>
+    <sheet name="m08" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'m05'!$A$1:$C$94</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'m06'!$A$1:$C$47</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="1048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1056">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -3173,6 +3174,30 @@
   </si>
   <si>
     <t>string id</t>
+  </si>
+  <si>
+    <t>dx_m08_5030_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_5020_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_5000_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_5010_darcy</t>
+  </si>
+  <si>
+    <t>0xa2cc80ca</t>
+  </si>
+  <si>
+    <t>0x82cc84cb</t>
+  </si>
+  <si>
+    <t>0x82ccccc9</t>
+  </si>
+  <si>
+    <t>0xa2ccc8c8</t>
   </si>
 </sst>
 </file>
@@ -7387,8 +7412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8544,4 +8569,91 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EEF99D-E35A-4C4E-B4B9-10A64AC19D37}">
+  <dimension ref="A1:F54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>859</v>
+      </c>
+      <c r="B1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C2" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C3" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C4" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mission 7 Space Voices. Mission 8 voices WIP
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B045911E-648C-4FA1-9007-D1EA3A2845B2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1EE622-FCB9-41FF-81B4-FB2907FCC558}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m01" sheetId="4" r:id="rId1"/>
@@ -19,18 +19,21 @@
     <sheet name="m04" sheetId="3" r:id="rId4"/>
     <sheet name="m05" sheetId="5" r:id="rId5"/>
     <sheet name="m06" sheetId="6" r:id="rId6"/>
-    <sheet name="m08" sheetId="7" r:id="rId7"/>
+    <sheet name="m07" sheetId="8" r:id="rId7"/>
+    <sheet name="m08" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'m05'!$A$1:$C$94</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'m06'!$A$1:$C$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'m07'!$A$1:$F$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'m08'!$A$1:$F$126</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="1056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="1463">
   <si>
     <t>DX_M02_0020_wilham</t>
   </si>
@@ -3198,6 +3201,1227 @@
   </si>
   <si>
     <t>0xa2ccc8c8</t>
+  </si>
+  <si>
+    <t>dx_m08_0000_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0005_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0010_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0020_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0030_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0040_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0050_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0060_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0070_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0080_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0090_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0100_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0110_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0120_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0130_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0140_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0150_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0160_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0170_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0180_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0190_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0200_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0210_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0220_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0230_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0240_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0250_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0260_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0270_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0280_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0290_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0300_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0310_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0320_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0330_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0340_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0350_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0360_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0370_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0380_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0390_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0400_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0410_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0420_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0430_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0440_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0450_captain</t>
+  </si>
+  <si>
+    <t>dx_m08_0460_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0470_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0480_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0490_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0500_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0510_captain</t>
+  </si>
+  <si>
+    <t>dx_m08_0520_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0530_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0540_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0550_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0560_captain</t>
+  </si>
+  <si>
+    <t>dx_m08_0570_tilton</t>
+  </si>
+  <si>
+    <t>dx_m08_0580_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0590_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0600_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0610_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0620_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0630_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0640_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0650_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0660_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0670_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0680_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0690_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0700_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0710_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0720_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0730_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0740_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0750_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0760_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0770_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0780_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0790_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0800_brighton</t>
+  </si>
+  <si>
+    <t>dx_m08_0810_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0820_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0830_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0840_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0850_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0860_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0870_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0880_red</t>
+  </si>
+  <si>
+    <t>dx_m08_0890_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0900_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0910_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0920_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0930_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0940_red</t>
+  </si>
+  <si>
+    <t>dx_m08_0950_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0960_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_0970_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_0980_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_0990_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1000_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_1010_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1020_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_1030_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1040_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_1050_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_1060_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_1070_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1080_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_1090_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1100_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_1110_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1120_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1130_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1140_hatcher</t>
+  </si>
+  <si>
+    <t>dx_m08_1150_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_1160_trent</t>
+  </si>
+  <si>
+    <t>dx_m08_1170_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_4900_darcy</t>
+  </si>
+  <si>
+    <t>dx_m08_4910_darcy</t>
+  </si>
+  <si>
+    <t>0x86c9aec9</t>
+  </si>
+  <si>
+    <t>0xab44c000</t>
+  </si>
+  <si>
+    <t>0xa6c9aac8</t>
+  </si>
+  <si>
+    <t>0xbb048082</t>
+  </si>
+  <si>
+    <t>0xa6c9e2ca</t>
+  </si>
+  <si>
+    <t>0xbb045884</t>
+  </si>
+  <si>
+    <t>0xa6c93acc</t>
+  </si>
+  <si>
+    <t>0xbb041086</t>
+  </si>
+  <si>
+    <t>0xa6c972ce</t>
+  </si>
+  <si>
+    <t>0xbb05e888</t>
+  </si>
+  <si>
+    <t>0x9b05ec89</t>
+  </si>
+  <si>
+    <t>0x86ddafc3</t>
+  </si>
+  <si>
+    <t>0x9b10cd8b</t>
+  </si>
+  <si>
+    <t>0x86dde7c1</t>
+  </si>
+  <si>
+    <t>0x9b108589</t>
+  </si>
+  <si>
+    <t>0x86dd3fc7</t>
+  </si>
+  <si>
+    <t>0xa266c1c6</t>
+  </si>
+  <si>
+    <t>0x86dd77c5</t>
+  </si>
+  <si>
+    <t>0x9b10158d</t>
+  </si>
+  <si>
+    <t>0xaf86c18d</t>
+  </si>
+  <si>
+    <t>0xa6dc8bca</t>
+  </si>
+  <si>
+    <t>0xbb4cca80</t>
+  </si>
+  <si>
+    <t>0xa681a8c8</t>
+  </si>
+  <si>
+    <t>0x8681e4cb</t>
+  </si>
+  <si>
+    <t>0x9b4c8683</t>
+  </si>
+  <si>
+    <t>0xbb4c5a84</t>
+  </si>
+  <si>
+    <t>0xa2677d06</t>
+  </si>
+  <si>
+    <t>0xa1677d0a</t>
+  </si>
+  <si>
+    <t>0x9b4c1687</t>
+  </si>
+  <si>
+    <t>0x86808cc1</t>
+  </si>
+  <si>
+    <t>0xa68088c0</t>
+  </si>
+  <si>
+    <t>0xbb58cb8a</t>
+  </si>
+  <si>
+    <t>0xa695a9c2</t>
+  </si>
+  <si>
+    <t>0xbb588388</t>
+  </si>
+  <si>
+    <t>0xa695e1c0</t>
+  </si>
+  <si>
+    <t>0xbb585b8e</t>
+  </si>
+  <si>
+    <t>0xa69539c6</t>
+  </si>
+  <si>
+    <t>0xbb58138c</t>
+  </si>
+  <si>
+    <t>0xa69571c4</t>
+  </si>
+  <si>
+    <t>0xbb59eb82</t>
+  </si>
+  <si>
+    <t>0x8aab4781</t>
+  </si>
+  <si>
+    <t>0xbb94cc80</t>
+  </si>
+  <si>
+    <t>0xa78c3981</t>
+  </si>
+  <si>
+    <t>0x8659e2cb</t>
+  </si>
+  <si>
+    <t>0x9b948083</t>
+  </si>
+  <si>
+    <t>0xa7083c8b</t>
+  </si>
+  <si>
+    <t>0x8a557b46</t>
+  </si>
+  <si>
+    <t>0xa7403e8b</t>
+  </si>
+  <si>
+    <t>0xa7543f81</t>
+  </si>
+  <si>
+    <t>0xa6b8308b</t>
+  </si>
+  <si>
+    <t>0xa6ac3181</t>
+  </si>
+  <si>
+    <t>0xb399328b</t>
+  </si>
+  <si>
+    <t>0x9b511342</t>
+  </si>
+  <si>
+    <t>0xb3d1308b</t>
+  </si>
+  <si>
+    <t>0xa64de7c0</t>
+  </si>
+  <si>
+    <t>0xbb805d8e</t>
+  </si>
+  <si>
+    <t>0xb31d3781</t>
+  </si>
+  <si>
+    <t>0xb7566542</t>
+  </si>
+  <si>
+    <t>0xb3553581</t>
+  </si>
+  <si>
+    <t>0x864c8bcb</t>
+  </si>
+  <si>
+    <t>0x9b81e983</t>
+  </si>
+  <si>
+    <t>0xa7056c06</t>
+  </si>
+  <si>
+    <t>0xa611acc8</t>
+  </si>
+  <si>
+    <t>0xa5056c0e</t>
+  </si>
+  <si>
+    <t>0x9bdc8283</t>
+  </si>
+  <si>
+    <t>0xa3656c03</t>
+  </si>
+  <si>
+    <t>0x9bdc5a85</t>
+  </si>
+  <si>
+    <t>0xa1656c0b</t>
+  </si>
+  <si>
+    <t>0xa0656c0f</t>
+  </si>
+  <si>
+    <t>0xaf856c4c</t>
+  </si>
+  <si>
+    <t>0xae856c48</t>
+  </si>
+  <si>
+    <t>0xbbc8cf8a</t>
+  </si>
+  <si>
+    <t>0xa605adc2</t>
+  </si>
+  <si>
+    <t>0xa505f84e</t>
+  </si>
+  <si>
+    <t>0x9bc88389</t>
+  </si>
+  <si>
+    <t>0x860539c7</t>
+  </si>
+  <si>
+    <t>0xa265f847</t>
+  </si>
+  <si>
+    <t>0x860571c5</t>
+  </si>
+  <si>
+    <t>0xa065f84f</t>
+  </si>
+  <si>
+    <t>0x860489cb</t>
+  </si>
+  <si>
+    <t>0xae85f808</t>
+  </si>
+  <si>
+    <t>0xa7027785</t>
+  </si>
+  <si>
+    <t>0xa7e9a2c8</t>
+  </si>
+  <si>
+    <t>0xba248882</t>
+  </si>
+  <si>
+    <t>0x9e98bbce</t>
+  </si>
+  <si>
+    <t>0xba245084</t>
+  </si>
+  <si>
+    <t>0xa69ec7ce</t>
+  </si>
+  <si>
+    <t>0xba241886</t>
+  </si>
+  <si>
+    <t>0x8e9cd3ce</t>
+  </si>
+  <si>
+    <t>0x9cc8edc3</t>
+  </si>
+  <si>
+    <t>0x96923fce</t>
+  </si>
+  <si>
+    <t>0x87fda7c3</t>
+  </si>
+  <si>
+    <t>0xa7fda3c2</t>
+  </si>
+  <si>
+    <t>0x8b99b1ca</t>
+  </si>
+  <si>
+    <t>0x9f98bbca</t>
+  </si>
+  <si>
+    <t>0x99d7ef49</t>
+  </si>
+  <si>
+    <t>0xa79ec7ca</t>
+  </si>
+  <si>
+    <t>0x87fd7fc5</t>
+  </si>
+  <si>
+    <t>0x8f9cd3ca</t>
+  </si>
+  <si>
+    <t>0xba31e182</t>
+  </si>
+  <si>
+    <t>0x97923fca</t>
+  </si>
+  <si>
+    <t>0x92c8a4c9</t>
+  </si>
+  <si>
+    <t>0xbe1a3bc4</t>
+  </si>
+  <si>
+    <t>0x92c8eccb</t>
+  </si>
+  <si>
+    <t>0x96182fc4</t>
+  </si>
+  <si>
+    <t>0xaf055284</t>
+  </si>
+  <si>
+    <t>0xb2c830cc</t>
+  </si>
+  <si>
+    <t>0xaf051a86</t>
+  </si>
+  <si>
+    <t>0x861c47c4</t>
+  </si>
+  <si>
+    <t>0xaf04e288</t>
+  </si>
+  <si>
+    <t>0x9e12abc4</t>
+  </si>
+  <si>
+    <t>0xaf11c38a</t>
+  </si>
+  <si>
+    <t>0xbf1a3bc0</t>
+  </si>
+  <si>
+    <t>0x831925c0</t>
+  </si>
+  <si>
+    <t>0x97182fc0</t>
+  </si>
+  <si>
+    <t>0xbb1f59c0</t>
+  </si>
+  <si>
+    <t>0xb2dc31c6</t>
+  </si>
+  <si>
+    <t>0xaf111b8c</t>
+  </si>
+  <si>
+    <t>0xb2dc79c4</t>
+  </si>
+  <si>
+    <t>0x97f9cfc3</t>
+  </si>
+  <si>
+    <t>0xb7f9cbc2</t>
+  </si>
+  <si>
+    <t>dx_m07_0010_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nЯ тут каких-то гопников раскидал, но Железного Зада среди них не было.</t>
+  </si>
+  <si>
+    <t>dx_m07_0020_barman</t>
+  </si>
+  <si>
+    <t>Бармен: Айронсайда, мистер Трент, Билла Айронсайда. Если его не было здесь, попробуйте во втором вероятном месте его пребывания. Скидываю координаты.</t>
+  </si>
+  <si>
+    <t>dx_m07_0030_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nСколько сколько прилетело? 500 кредитов? Они тут совсем охренели?</t>
+  </si>
+  <si>
+    <t>dx_m07_0035_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nПроще было вообще перевод не делать - на банковской комиссии больше потеряли. Стоит, пожалуй, еще пару вопросов этому бармену задать. Например, "где деньги, Лебовски?".</t>
+  </si>
+  <si>
+    <t>dx_m07_0040_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд: Мистер Трент, меня зовут Рокфорд, СБА прислало меня помочь вам в поиске артефактов. Жду вас в баре на планете Кадиз. Прошу вас быть как можно скорее, счет идет на секунды.</t>
+  </si>
+  <si>
+    <t>dx_m07_0060_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nТрент, жить хочешь? Помогай!</t>
+  </si>
+  <si>
+    <t>dx_m07_0070_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nТрент, теперь за мной в торговую линию! Сначала летим к Гаване, затем к гипервратам в Малый Омикрон.</t>
+  </si>
+  <si>
+    <t>dx_m07_0080_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nПриятно познакомиться, мистер Рокфорд.</t>
+  </si>
+  <si>
+    <t>dx_m07_0090_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nНе мистер. Просто Рокфорд.</t>
+  </si>
+  <si>
+    <t>dx_m07_0100_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nКто были все эти люди, Рокфорд?</t>
+  </si>
+  <si>
+    <t>dx_m07_0110_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nАгенты Ордена.</t>
+  </si>
+  <si>
+    <t>dx_m07_0120_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nА можно поподробнее?</t>
+  </si>
+  <si>
+    <t>dx_m07_0130_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nО чем?</t>
+  </si>
+  <si>
+    <t>dx_m07_0140_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nВообще о многом. Если вкратце, кто вы и во что я в очередной раз вляпался.</t>
+  </si>
+  <si>
+    <t>dx_m07_0150_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nЯ агент СБА Рокфорд и меня прислали на помощь группе Дельта и вам, Трент, потому что вы вляпались в неприятности.</t>
+  </si>
+  <si>
+    <t>dx_m07_0160_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nДа твою же налево... Хорошо, тогда расскажите более развернуто, как вы меня нашли, почему вас, то есть нас на Кадизе ждали, и что вообще мы теперь планируем делать.</t>
+  </si>
+  <si>
+    <t>dx_m07_0170_rockford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рокфорд:\nКогда я прибыл в систему Кадиз, я вышел на связь с лидером Дельта и узнал от него о сложившейся ситуации и о том, что боеспособный корабль остался только у вас. </t>
+  </si>
+  <si>
+    <t>dx_m07_0180_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nЯ отследил все взятые в этой системе фриленсерами контракты и определил ваше местонахождение. Кстати, Трент, вы действительно готовы работать за такие гроши?</t>
+  </si>
+  <si>
+    <t>dx_m07_0190_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nНе будем об этом. Что было дальше?</t>
+  </si>
+  <si>
+    <t>dx_m07_0200_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nЯ знал что за вами следят агенты Ордена. Кроме того, они подозревали о моем присутствии в системе.</t>
+  </si>
+  <si>
+    <t>dx_m07_0210_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nПоэтому я решил устроить им ловушку и послал вам сообщение с просьбой о встрече в максимально удаленной от их главных сил точке - на планете Кадиз.</t>
+  </si>
+  <si>
+    <t>dx_m07_0220_rockford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рокфорд:\nОни смогли отправить на Кадиз только небольшую группу перехвата, а мы с вами, Трент смогли ее уничтожить. Насчет того, что делать дальше, по-моему очевидно, забирать артефакты. </t>
+  </si>
+  <si>
+    <t>dx_m07_0230_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nИ у нас уже есть план?</t>
+  </si>
+  <si>
+    <t>dx_m07_0240_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nКонечно. Как можно лететь куда-то без плана?</t>
+  </si>
+  <si>
+    <t>dx_m07_0250_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nМеня в него не посветите?</t>
+  </si>
+  <si>
+    <t>dx_m07_0260_rockford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рокфорд:\nАртефакты содержатся на базе Тортуга в системе Малый Омикрон. Формально это пиратская база, но она используется агентами Ордена и поэтому отлично защищена. </t>
+  </si>
+  <si>
+    <t>dx_m07_0270_rockford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рокфорд:\nНа станции находится передатчик, обеспечивающий постоянную двустороннюю связь со штабом Ордена. </t>
+  </si>
+  <si>
+    <t>dx_m07_0280_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nЕсли передатчик будет выведен из строя, по протоколу они обязаны эвакуировать все важные объекты на ближайшую другую базу. Мы разрушим передатчик и нападем на конвой, перевозящий артефакты.</t>
+  </si>
+  <si>
+    <t>dx_m07_0290_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nЭмм... Ну ты у нас тут специалист, тебе виднее. Кстати, Рокфорд, а почему тебя так хотят убить агенты Ордена? Стоило тебе выйти на связь и на место встречи прибыла целая армия.</t>
+  </si>
+  <si>
+    <t>dx_m07_0300_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nЯ был агентом еще старого, большого Ордена. Я слишком много знаю. С момента раскола постоянно приходится спать вполглаза.</t>
+  </si>
+  <si>
+    <t>dx_m07_0310_rockford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рокфорд:\nСейчас я сброшу контейнеры с зарядами направленного действия. Подберите их, Трент, расположите вокруг передатчика и подорвите. </t>
+  </si>
+  <si>
+    <t>dx_m07_0320_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nУстанавливайте заряды с выключенным щитом, иначе они сдетонируют. Координаты передатчика в вашем компьютере. Вперед!</t>
+  </si>
+  <si>
+    <t>dx_m07_0330_tortuga</t>
+  </si>
+  <si>
+    <t>dx_m07_0340_tortuga</t>
+  </si>
+  <si>
+    <t>dx_m07_0350_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nГотово. Передатчик уничтожен.</t>
+  </si>
+  <si>
+    <t>dx_m07_0360_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nВижу конвой выходящий из Тортуги. Направляюсь за ним. Передаю координаты.</t>
+  </si>
+  <si>
+    <t>dx_m07_0370_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nПерехватываю грузовик. Нужна помощь.</t>
+  </si>
+  <si>
+    <t>dx_m07_0380_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nТрент, атакуйте грузовик!</t>
+  </si>
+  <si>
+    <t>dx_m07_0390_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nЩит грузовика просто непробиваем. Что делать то?</t>
+  </si>
+  <si>
+    <t>dx_m07_0400_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nТрент, частое использование Электромагнитной пушки приведет к перегреву генераторов и отключению щита. Подлети ближе к транспорту, чтобы пилот мог по тебе стрелять.</t>
+  </si>
+  <si>
+    <t>dx_m07_0410_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nВ смысле? Быть приманкой?</t>
+  </si>
+  <si>
+    <t>dx_m07_0420_rockford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рокфорд:\nДа. </t>
+  </si>
+  <si>
+    <t>dx_m07_0430_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nЩит упал. Трент, уничтожь грузовик!</t>
+  </si>
+  <si>
+    <t>dx_m07_0440_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nТрент, пилот грузовика запускает гипердвигатель. Уничтожь грузовик! Быстрее!</t>
+  </si>
+  <si>
+    <t>dx_m07_0450_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nЭто было потно. Куда теперь?</t>
+  </si>
+  <si>
+    <t>dx_m07_0460_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nУ меня есть убежище в Омега-13. Проведем там обслуживание кораблей и разработаем план доставки артефактов в штаб СБА.</t>
+  </si>
+  <si>
+    <t>dx_m07_0470_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nЗвучит отлично! Веди. Кстати, а что попалось тебе? У меня какая-то мелочевка кочевников и том Протея... Значит ключ у тебя?</t>
+  </si>
+  <si>
+    <t>dx_m07_0480_rockford</t>
+  </si>
+  <si>
+    <t>Рокфорд:\nДа.</t>
+  </si>
+  <si>
+    <t>dx_m07_0500_trent</t>
+  </si>
+  <si>
+    <t>Трент:\nНужно добраться до ближайшей базы.</t>
+  </si>
+  <si>
+    <t>dx_m07_0510_darcy</t>
+  </si>
+  <si>
+    <t>Дерси:\nДавай, шутник, залетай в торговую линию. Тут лететь не далеко.</t>
+  </si>
+  <si>
+    <t>dx_m07_0520_darcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дерси:\nТы там особо с ним не откровенничай. Эта личность чрезвычайно мутная. </t>
+  </si>
+  <si>
+    <t>dx_m07_0530_darcy</t>
+  </si>
+  <si>
+    <t>Дерси:\nОн часто бывает нам полезен, поэтому мы закрываем глаза на его мелкие шалости, но, чует мое сердце, до поры до времени. Когда-нибудь он нарвется.</t>
+  </si>
+  <si>
+    <t>dx_m07_0550_bandit</t>
+  </si>
+  <si>
+    <t>Бандит:\nФриленсер, у тебя есть кое-что что, что очень нужно нам. Отдай по-хорошему!</t>
+  </si>
+  <si>
+    <t>dx_m07_0560_darcy</t>
+  </si>
+  <si>
+    <t>Дерси:\nМальчики, а вы не охренели? Это мой участок, я здесь главный коп. Трент, давай разберем эту шпану. dx_m07_0570_darcy</t>
+  </si>
+  <si>
+    <t>Дерси:\nДжабба, засранец, теперь ты точно доигрался. Трент, я вернусь, поговорю с нашим другом еще раз. Увидимся на станции.</t>
+  </si>
+  <si>
+    <t>dx_m07_0570_darcy</t>
+  </si>
+  <si>
+    <t>0x9b034342</t>
+  </si>
+  <si>
+    <t>0x95582189</t>
+  </si>
+  <si>
+    <t>0x9b030b40</t>
+  </si>
+  <si>
+    <t>0x8b4303c0</t>
+  </si>
+  <si>
+    <t>0xa25e0447</t>
+  </si>
+  <si>
+    <t>0xa05e044f</t>
+  </si>
+  <si>
+    <t>0xa15e044b</t>
+  </si>
+  <si>
+    <t>0xbb02674b</t>
+  </si>
+  <si>
+    <t>0xafbe040c</t>
+  </si>
+  <si>
+    <t>0xbb174649</t>
+  </si>
+  <si>
+    <t>0xa73e9006</t>
+  </si>
+  <si>
+    <t>0xbb170e4b</t>
+  </si>
+  <si>
+    <t>0xa53e900e</t>
+  </si>
+  <si>
+    <t>0xbb17d64d</t>
+  </si>
+  <si>
+    <t>0xa35e9003</t>
+  </si>
+  <si>
+    <t>0xbb179e4f</t>
+  </si>
+  <si>
+    <t>0xa15e900b</t>
+  </si>
+  <si>
+    <t>0xaebe9048</t>
+  </si>
+  <si>
+    <t>0x9b166240</t>
+  </si>
+  <si>
+    <t>0xa63f2cc2</t>
+  </si>
+  <si>
+    <t>0xa73f2cc6</t>
+  </si>
+  <si>
+    <t>0xa43f2cca</t>
+  </si>
+  <si>
+    <t>0x9b4b0940</t>
+  </si>
+  <si>
+    <t>0xa25f2cc7</t>
+  </si>
+  <si>
+    <t>0x9b4bd146</t>
+  </si>
+  <si>
+    <t>0xa05f2ccf</t>
+  </si>
+  <si>
+    <t>0xa15f2ccb</t>
+  </si>
+  <si>
+    <t>0xaebf2c88</t>
+  </si>
+  <si>
+    <t>0x9b4a614a</t>
+  </si>
+  <si>
+    <t>0xa63fb882</t>
+  </si>
+  <si>
+    <t>0xa73fb886</t>
+  </si>
+  <si>
+    <t>0xa43fb88a</t>
+  </si>
+  <si>
+    <t>0x95bfbc81</t>
+  </si>
+  <si>
+    <t>0xb9b8ca81</t>
+  </si>
+  <si>
+    <t>0x9b5fd04c</t>
+  </si>
+  <si>
+    <t>0xa05fb88f</t>
+  </si>
+  <si>
+    <t>0xa15fb88b</t>
+  </si>
+  <si>
+    <t>0xaebfb8c8</t>
+  </si>
+  <si>
+    <t>0x9b5e6040</t>
+  </si>
+  <si>
+    <t>0xa63c1543</t>
+  </si>
+  <si>
+    <t>0x9b934742</t>
+  </si>
+  <si>
+    <t>0xa43c154b</t>
+  </si>
+  <si>
+    <t>0xa53c154f</t>
+  </si>
+  <si>
+    <t>0xa25c1546</t>
+  </si>
+  <si>
+    <t>0x9b93d746</t>
+  </si>
+  <si>
+    <t>0xa05c154e</t>
+  </si>
+  <si>
+    <t>0x9b939f44</t>
+  </si>
+  <si>
+    <t>0xaebc1509</t>
+  </si>
+  <si>
+    <t>0xbb874249</t>
+  </si>
+  <si>
+    <t>0xa64a2001</t>
+  </si>
+  <si>
+    <t>0x864a6c02</t>
+  </si>
+  <si>
+    <t>0xa64a6803</t>
+  </si>
+  <si>
+    <t>0xb4f216cd</t>
+  </si>
+  <si>
+    <t>0x864afc06</t>
+  </si>
+  <si>
+    <t>0xa64af807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Диспетчер станции:\nФриленсер альфа-один, немедленно покиньте запретную зону... </t>
+  </si>
+  <si>
+    <t>Диспетчер станции:\nФриленсер альфа-один, если вы не покинете зону, мы будем вынуждены активировать защитный периметр!</t>
   </si>
 </sst>
 </file>
@@ -8572,11 +9796,829 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EEF99D-E35A-4C4E-B4B9-10A64AC19D37}">
-  <dimension ref="A1:F54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0A17A6-8B3A-4227-8855-14263B4C06B6}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="F48" sqref="F48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>859</v>
+      </c>
+      <c r="B1" t="s">
+        <v>860</v>
+      </c>
+      <c r="C1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C2" t="s">
+        <v>863</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C3" t="s">
+        <v>864</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C4" t="s">
+        <v>863</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C5" t="s">
+        <v>863</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C6" t="s">
+        <v>864</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C7" t="s">
+        <v>864</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C8" t="s">
+        <v>864</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C9" t="s">
+        <v>863</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C10" t="s">
+        <v>864</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C11" t="s">
+        <v>863</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C12" t="s">
+        <v>864</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C13" t="s">
+        <v>863</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C14" t="s">
+        <v>864</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C15" t="s">
+        <v>863</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C16" t="s">
+        <v>864</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C17" t="s">
+        <v>863</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C18" t="s">
+        <v>864</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C19" t="s">
+        <v>864</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C20" t="s">
+        <v>863</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C21" t="s">
+        <v>864</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C22" t="s">
+        <v>864</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C23" t="s">
+        <v>864</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C24" t="s">
+        <v>863</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C25" t="s">
+        <v>864</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C26" t="s">
+        <v>863</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C27" t="s">
+        <v>864</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C28" t="s">
+        <v>864</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C29" t="s">
+        <v>864</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C30" t="s">
+        <v>863</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C31" t="s">
+        <v>864</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C32" t="s">
+        <v>864</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C33" t="s">
+        <v>864</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C34" t="s">
+        <v>864</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C35" t="s">
+        <v>864</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C36" t="s">
+        <v>863</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C37" t="s">
+        <v>864</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C38" t="s">
+        <v>864</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C39" t="s">
+        <v>864</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C40" t="s">
+        <v>863</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C41" t="s">
+        <v>864</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C42" t="s">
+        <v>863</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C43" t="s">
+        <v>864</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C44" t="s">
+        <v>864</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C45" t="s">
+        <v>864</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C46" t="s">
+        <v>863</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C47" t="s">
+        <v>864</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C48" t="s">
+        <v>863</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C49" t="s">
+        <v>864</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C50" t="s">
+        <v>863</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C51" t="s">
+        <v>862</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C52" t="s">
+        <v>862</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C53" t="s">
+        <v>862</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C54" t="s">
+        <v>864</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C55" t="s">
+        <v>862</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C56" t="s">
+        <v>862</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F56" xr:uid="{50B42C78-4DD3-4C40-ACA1-9DC6BAC0BC09}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="trent"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EEF99D-E35A-4C4E-B4B9-10A64AC19D37}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F126"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8605,12 +10647,12 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="B2" t="s">
-        <v>1054</v>
+        <v>1177</v>
       </c>
       <c r="C2" t="s">
         <v>862</v>
@@ -8618,21 +10660,21 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1051</v>
+        <v>1057</v>
       </c>
       <c r="B3" t="s">
-        <v>1055</v>
+        <v>1178</v>
       </c>
       <c r="C3" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1049</v>
+        <v>1058</v>
       </c>
       <c r="B4" t="s">
-        <v>1053</v>
+        <v>1179</v>
       </c>
       <c r="C4" t="s">
         <v>862</v>
@@ -8640,19 +10682,1355 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C6" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C7" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C8" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C10" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C11" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C12" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C13" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C14" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C15" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C16" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C17" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C18" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C19" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C20" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C21" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C22" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C23" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C24" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C25" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C26" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C27" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C28" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C29" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C30" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C31" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C32" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C33" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C34" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C35" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C36" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C37" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C38" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C39" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C40" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C41" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C42" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C43" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C44" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C45" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C46" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C47" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C48" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C49" t="s">
+        <v>864</v>
+      </c>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C50" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C51" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C52" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C53" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C54" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C55" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C56" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C57" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C58" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C59" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C60" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C61" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C62" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C63" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C64" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C65" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C66" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C67" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C68" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C69" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C70" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C71" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C72" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C73" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C74" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C75" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C76" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C77" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C78" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C79" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C80" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C81" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C82" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C83" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C84" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C85" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C86" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C87" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C88" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C89" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C90" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C91" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C92" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C93" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C94" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C95" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C96" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C97" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C98" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C99" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C100" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C101" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C102" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C103" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C104" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C105" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C106" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C107" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C108" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C109" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C110" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C111" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C112" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C113" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C114" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C115" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C116" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C117" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C118" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C119" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C120" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C121" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C122" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C123" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C124" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C125" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>1048</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B126" t="s">
         <v>1052</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C126" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F54" s="4"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:F126" xr:uid="{CEAE1525-0CA8-45C3-8F69-CA8FEDD7D6A1}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="trent"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Mission 7 Work in progress
</commit_message>
<xml_diff>
--- a/Assets/AUDIO_XML_RU/voices.xlsx
+++ b/Assets/AUDIO_XML_RU/voices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Freelancer Game\FL_MOD\Assets\AUDIO_XML_RU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1EE622-FCB9-41FF-81B4-FB2907FCC558}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339E7CC-E848-409B-B1C0-716B2E31B47B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18525" windowHeight="12210" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4428,8 +4428,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -4458,7 +4467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -4470,6 +4479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -9797,11 +9807,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B0A17A6-8B3A-4227-8855-14263B4C06B6}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9844,7 +9853,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1300</v>
       </c>
@@ -9886,7 +9895,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1306</v>
       </c>
@@ -9900,7 +9909,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1308</v>
       </c>
@@ -9914,7 +9923,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1310</v>
       </c>
@@ -9942,7 +9951,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1314</v>
       </c>
@@ -9970,7 +9979,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1318</v>
       </c>
@@ -9998,7 +10007,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1322</v>
       </c>
@@ -10026,7 +10035,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1326</v>
       </c>
@@ -10036,7 +10045,7 @@
       <c r="C16" t="s">
         <v>864</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>1327</v>
       </c>
     </row>
@@ -10050,11 +10059,11 @@
       <c r="C17" t="s">
         <v>863</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="5" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1330</v>
       </c>
@@ -10068,7 +10077,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1332</v>
       </c>
@@ -10096,7 +10105,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1336</v>
       </c>
@@ -10110,7 +10119,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1338</v>
       </c>
@@ -10124,7 +10133,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1340</v>
       </c>
@@ -10152,7 +10161,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1344</v>
       </c>
@@ -10180,7 +10189,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1348</v>
       </c>
@@ -10194,7 +10203,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1350</v>
       </c>
@@ -10208,7 +10217,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1352</v>
       </c>
@@ -10236,7 +10245,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1356</v>
       </c>
@@ -10250,7 +10259,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1358</v>
       </c>
@@ -10264,7 +10273,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1360</v>
       </c>
@@ -10278,7 +10287,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1362</v>
       </c>
@@ -10292,7 +10301,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1363</v>
       </c>
@@ -10320,7 +10329,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1366</v>
       </c>
@@ -10334,7 +10343,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1368</v>
       </c>
@@ -10348,7 +10357,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1370</v>
       </c>
@@ -10376,7 +10385,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1374</v>
       </c>
@@ -10404,7 +10413,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1378</v>
       </c>
@@ -10418,7 +10427,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1380</v>
       </c>
@@ -10432,7 +10441,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1382</v>
       </c>
@@ -10460,7 +10469,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1386</v>
       </c>
@@ -10488,7 +10497,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1390</v>
       </c>
@@ -10516,7 +10525,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1394</v>
       </c>
@@ -10530,7 +10539,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>1396</v>
       </c>
@@ -10544,7 +10553,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1398</v>
       </c>
@@ -10558,7 +10567,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1400</v>
       </c>
@@ -10572,7 +10581,7 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>1402</v>
       </c>
@@ -10586,7 +10595,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1405</v>
       </c>
@@ -10601,14 +10610,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F56" xr:uid="{50B42C78-4DD3-4C40-ACA1-9DC6BAC0BC09}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="trent"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F56" xr:uid="{50B42C78-4DD3-4C40-ACA1-9DC6BAC0BC09}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10618,7 +10622,7 @@
   <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10647,7 +10651,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1056</v>
       </c>
@@ -10658,7 +10662,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1057</v>
       </c>
@@ -10669,7 +10673,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1058</v>
       </c>
@@ -10680,7 +10684,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1059</v>
       </c>
@@ -10691,7 +10695,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1060</v>
       </c>
@@ -10702,7 +10706,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1061</v>
       </c>
@@ -10713,7 +10717,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1062</v>
       </c>
@@ -10724,7 +10728,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1063</v>
       </c>
@@ -10735,7 +10739,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1064</v>
       </c>
@@ -10746,7 +10750,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1065</v>
       </c>
@@ -10757,7 +10761,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1066</v>
       </c>
@@ -10768,7 +10772,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1067</v>
       </c>
@@ -10779,7 +10783,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1068</v>
       </c>
@@ -10790,7 +10794,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1069</v>
       </c>
@@ -10801,7 +10805,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1070</v>
       </c>
@@ -10812,7 +10816,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1071</v>
       </c>
@@ -10834,7 +10838,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1073</v>
       </c>
@@ -10845,7 +10849,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1074</v>
       </c>
@@ -10867,7 +10871,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1076</v>
       </c>
@@ -10878,7 +10882,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1077</v>
       </c>
@@ -10889,7 +10893,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1078</v>
       </c>
@@ -10900,7 +10904,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1079</v>
       </c>
@@ -10911,7 +10915,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1080</v>
       </c>
@@ -10922,7 +10926,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1081</v>
       </c>
@@ -10955,7 +10959,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1084</v>
       </c>
@@ -10966,7 +10970,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1085</v>
       </c>
@@ -10977,7 +10981,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1086</v>
       </c>
@@ -10988,7 +10992,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1087</v>
       </c>
@@ -10999,7 +11003,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1088</v>
       </c>
@@ -11010,7 +11014,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1089</v>
       </c>
@@ -11021,7 +11025,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1090</v>
       </c>
@@ -11032,7 +11036,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1091</v>
       </c>
@@ -11043,7 +11047,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1092</v>
       </c>
@@ -11054,7 +11058,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1093</v>
       </c>
@@ -11065,7 +11069,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1094</v>
       </c>
@@ -11076,7 +11080,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1095</v>
       </c>
@@ -11098,7 +11102,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1097</v>
       </c>
@@ -11120,7 +11124,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1099</v>
       </c>
@@ -11131,7 +11135,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1100</v>
       </c>
@@ -11242,7 +11246,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>1110</v>
       </c>
@@ -11253,7 +11257,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>1111</v>
       </c>
@@ -11297,7 +11301,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>1115</v>
       </c>
@@ -11308,7 +11312,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1116</v>
       </c>
@@ -11330,7 +11334,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>1118</v>
       </c>
@@ -11352,7 +11356,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1120</v>
       </c>
@@ -11374,7 +11378,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1122</v>
       </c>
@@ -11429,7 +11433,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1127</v>
       </c>
@@ -11440,7 +11444,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1128</v>
       </c>
@@ -11462,7 +11466,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1130</v>
       </c>
@@ -11473,7 +11477,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1131</v>
       </c>
@@ -11495,7 +11499,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1133</v>
       </c>
@@ -11517,7 +11521,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1135</v>
       </c>
@@ -11550,7 +11554,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1138</v>
       </c>
@@ -11561,7 +11565,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1139</v>
       </c>
@@ -11572,7 +11576,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1140</v>
       </c>
@@ -11583,7 +11587,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1141</v>
       </c>
@@ -11594,7 +11598,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1142</v>
       </c>
@@ -11605,7 +11609,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1143</v>
       </c>
@@ -11616,7 +11620,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1144</v>
       </c>
@@ -11638,7 +11642,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1146</v>
       </c>
@@ -11649,7 +11653,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1147</v>
       </c>
@@ -11660,7 +11664,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1148</v>
       </c>
@@ -11671,7 +11675,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1149</v>
       </c>
@@ -11682,7 +11686,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1150</v>
       </c>
@@ -11704,7 +11708,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1152</v>
       </c>
@@ -11715,7 +11719,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1153</v>
       </c>
@@ -11726,7 +11730,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1154</v>
       </c>
@@ -11737,7 +11741,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1155</v>
       </c>
@@ -11748,7 +11752,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1156</v>
       </c>
@@ -11759,7 +11763,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1157</v>
       </c>
@@ -11770,7 +11774,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1158</v>
       </c>
@@ -11781,7 +11785,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1159</v>
       </c>
@@ -11792,7 +11796,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1160</v>
       </c>
@@ -11803,7 +11807,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1161</v>
       </c>
@@ -11814,7 +11818,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1162</v>
       </c>
@@ -11825,7 +11829,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1163</v>
       </c>
@@ -11836,7 +11840,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1164</v>
       </c>
@@ -11847,7 +11851,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1165</v>
       </c>
@@ -11858,7 +11862,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1166</v>
       </c>
@@ -11869,7 +11873,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1167</v>
       </c>
@@ -11880,7 +11884,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1168</v>
       </c>
@@ -11891,7 +11895,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1169</v>
       </c>
@@ -11902,7 +11906,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1170</v>
       </c>
@@ -11913,7 +11917,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>1171</v>
       </c>
@@ -11924,7 +11928,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>1172</v>
       </c>
@@ -11935,7 +11939,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>1173</v>
       </c>
@@ -11946,7 +11950,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>1174</v>
       </c>
@@ -11957,7 +11961,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>1175</v>
       </c>
@@ -11968,7 +11972,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1176</v>
       </c>
@@ -11979,7 +11983,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1050</v>
       </c>
@@ -11990,7 +11994,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>1051</v>
       </c>
@@ -12001,7 +12005,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>1049</v>
       </c>
@@ -12012,7 +12016,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1048</v>
       </c>
@@ -12027,7 +12031,7 @@
   <autoFilter ref="A1:F126" xr:uid="{CEAE1525-0CA8-45C3-8F69-CA8FEDD7D6A1}">
     <filterColumn colId="2">
       <filters>
-        <filter val="trent"/>
+        <filter val="female"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>